<commit_message>
Updated names for forms, and renamed 'Request Form' to 'Form'
</commit_message>
<xml_diff>
--- a/rdepart.xlsx
+++ b/rdepart.xlsx
@@ -147,7 +147,7 @@
     <t>form_id</t>
   </si>
   <si>
-    <t>Results Pickup</t>
+    <t>3. Results Pickup</t>
   </si>
   <si>
     <t>rdepart</t>
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -228,6 +228,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -392,13 +395,13 @@
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="6"/>
@@ -442,29 +445,29 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
@@ -524,7 +527,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -539,18 +542,18 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add additional facilities, sample type, and add sample ID barcode validation
</commit_message>
<xml_diff>
--- a/rdepart.xlsx
+++ b/rdepart.xlsx
@@ -13,21 +13,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+  <si>
+    <t>list name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>list name</t>
+    <t>region</t>
   </si>
   <si>
     <t>required</t>
@@ -39,75 +42,78 @@
     <t>calculation</t>
   </si>
   <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>lab_key</t>
+  </si>
+  <si>
+    <t>constraint message</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>facility</t>
+  </si>
+  <si>
+    <t>facility_key</t>
+  </si>
+  <si>
+    <t>stype</t>
+  </si>
+  <si>
     <t>start</t>
   </si>
   <si>
+    <t>stype_key</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>cond_key</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>deviceid</t>
+  </si>
+  <si>
+    <t>simserial</t>
+  </si>
+  <si>
+    <t>select_one region</t>
+  </si>
+  <si>
     <t>form_id</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>deviceid</t>
-  </si>
-  <si>
-    <t>simserial</t>
-  </si>
-  <si>
     <t>3. Results Pickup</t>
   </si>
   <si>
-    <t>select_one region</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
     <t>Facility Lab</t>
   </si>
   <si>
-    <t>lab_key</t>
+    <t>rdepart</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>lab</t>
-  </si>
-  <si>
     <t>quick search('labs')</t>
   </si>
   <si>
-    <t>facility</t>
-  </si>
-  <si>
-    <t>facility_key</t>
-  </si>
-  <si>
     <t>calculate</t>
   </si>
   <si>
-    <t>stype</t>
-  </si>
-  <si>
-    <t>stype_key</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>cond_key</t>
-  </si>
-  <si>
-    <t>cond</t>
-  </si>
-  <si>
-    <t>rdepart</t>
-  </si>
-  <si>
     <t>pulldata('facilities', 'facility_key', 'facility_key', ${region})</t>
   </si>
   <si>
@@ -127,6 +133,12 @@
   </si>
   <si>
     <t>STT Barcode</t>
+  </si>
+  <si>
+    <t>regex(., '[\w\d]{9}\d{3}')</t>
+  </si>
+  <si>
+    <t>Scanned barcode does not match the required pattern</t>
   </si>
   <si>
     <t>end repeat</t>
@@ -153,20 +165,20 @@
     </font>
     <font>
       <b/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
     <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -197,47 +209,53 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -271,3149 +289,3179 @@
     <col customWidth="1" min="3" max="3" width="23.71"/>
     <col customWidth="1" min="5" max="5" width="16.71"/>
     <col customWidth="1" min="6" max="6" width="46.14"/>
+    <col customWidth="1" min="7" max="7" width="19.71"/>
+    <col customWidth="1" min="8" max="8" width="45.43"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="C6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="5"/>
+      <c r="B9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="5"/>
+      <c r="A10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12">
-      <c r="F12" s="5"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13">
-      <c r="F13" s="5"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14">
-      <c r="F14" s="5"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15">
-      <c r="F15" s="5"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16">
-      <c r="F16" s="5"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17">
-      <c r="F17" s="5"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18">
-      <c r="F18" s="5"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19">
-      <c r="F19" s="5"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20">
-      <c r="F20" s="5"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21">
-      <c r="F21" s="5"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22">
-      <c r="F22" s="5"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23">
-      <c r="F23" s="5"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24">
-      <c r="F24" s="5"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25">
-      <c r="F25" s="5"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26">
-      <c r="F26" s="5"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27">
-      <c r="F27" s="5"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28">
-      <c r="F28" s="5"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29">
-      <c r="F29" s="5"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30">
-      <c r="F30" s="5"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31">
-      <c r="F31" s="5"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32">
-      <c r="F32" s="5"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33">
-      <c r="F33" s="5"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34">
-      <c r="F34" s="5"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35">
-      <c r="F35" s="5"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36">
-      <c r="F36" s="5"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37">
-      <c r="F37" s="5"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38">
-      <c r="F38" s="5"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39">
-      <c r="F39" s="5"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40">
-      <c r="F40" s="5"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41">
-      <c r="F41" s="5"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42">
-      <c r="F42" s="5"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43">
-      <c r="F43" s="5"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44">
-      <c r="F44" s="5"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45">
-      <c r="F45" s="5"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46">
-      <c r="F46" s="5"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47">
-      <c r="F47" s="5"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48">
-      <c r="F48" s="5"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49">
-      <c r="F49" s="5"/>
+      <c r="F49" s="10"/>
     </row>
     <row r="50">
-      <c r="F50" s="5"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51">
-      <c r="F51" s="5"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="52">
-      <c r="F52" s="5"/>
+      <c r="F52" s="10"/>
     </row>
     <row r="53">
-      <c r="F53" s="5"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54">
-      <c r="F54" s="5"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55">
-      <c r="F55" s="5"/>
+      <c r="F55" s="10"/>
     </row>
     <row r="56">
-      <c r="F56" s="5"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57">
-      <c r="F57" s="5"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58">
-      <c r="F58" s="5"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="59">
-      <c r="F59" s="5"/>
+      <c r="F59" s="10"/>
     </row>
     <row r="60">
-      <c r="F60" s="5"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="61">
-      <c r="F61" s="5"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62">
-      <c r="F62" s="5"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63">
-      <c r="F63" s="5"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64">
-      <c r="F64" s="5"/>
+      <c r="F64" s="10"/>
     </row>
     <row r="65">
-      <c r="F65" s="5"/>
+      <c r="F65" s="10"/>
     </row>
     <row r="66">
-      <c r="F66" s="5"/>
+      <c r="F66" s="10"/>
     </row>
     <row r="67">
-      <c r="F67" s="5"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68">
-      <c r="F68" s="5"/>
+      <c r="F68" s="10"/>
     </row>
     <row r="69">
-      <c r="F69" s="5"/>
+      <c r="F69" s="10"/>
     </row>
     <row r="70">
-      <c r="F70" s="5"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71">
-      <c r="F71" s="5"/>
+      <c r="F71" s="10"/>
     </row>
     <row r="72">
-      <c r="F72" s="5"/>
+      <c r="F72" s="10"/>
     </row>
     <row r="73">
-      <c r="F73" s="5"/>
+      <c r="F73" s="10"/>
     </row>
     <row r="74">
-      <c r="F74" s="5"/>
+      <c r="F74" s="10"/>
     </row>
     <row r="75">
-      <c r="F75" s="5"/>
+      <c r="F75" s="10"/>
     </row>
     <row r="76">
-      <c r="F76" s="5"/>
+      <c r="F76" s="10"/>
     </row>
     <row r="77">
-      <c r="F77" s="5"/>
+      <c r="F77" s="10"/>
     </row>
     <row r="78">
-      <c r="F78" s="5"/>
+      <c r="F78" s="10"/>
     </row>
     <row r="79">
-      <c r="F79" s="5"/>
+      <c r="F79" s="10"/>
     </row>
     <row r="80">
-      <c r="F80" s="5"/>
+      <c r="F80" s="10"/>
     </row>
     <row r="81">
-      <c r="F81" s="5"/>
+      <c r="F81" s="10"/>
     </row>
     <row r="82">
-      <c r="F82" s="5"/>
+      <c r="F82" s="10"/>
     </row>
     <row r="83">
-      <c r="F83" s="5"/>
+      <c r="F83" s="10"/>
     </row>
     <row r="84">
-      <c r="F84" s="5"/>
+      <c r="F84" s="10"/>
     </row>
     <row r="85">
-      <c r="F85" s="5"/>
+      <c r="F85" s="10"/>
     </row>
     <row r="86">
-      <c r="F86" s="5"/>
+      <c r="F86" s="10"/>
     </row>
     <row r="87">
-      <c r="F87" s="5"/>
+      <c r="F87" s="10"/>
     </row>
     <row r="88">
-      <c r="F88" s="5"/>
+      <c r="F88" s="10"/>
     </row>
     <row r="89">
-      <c r="F89" s="5"/>
+      <c r="F89" s="10"/>
     </row>
     <row r="90">
-      <c r="F90" s="5"/>
+      <c r="F90" s="10"/>
     </row>
     <row r="91">
-      <c r="F91" s="5"/>
+      <c r="F91" s="10"/>
     </row>
     <row r="92">
-      <c r="F92" s="5"/>
+      <c r="F92" s="10"/>
     </row>
     <row r="93">
-      <c r="F93" s="5"/>
+      <c r="F93" s="10"/>
     </row>
     <row r="94">
-      <c r="F94" s="5"/>
+      <c r="F94" s="10"/>
     </row>
     <row r="95">
-      <c r="F95" s="5"/>
+      <c r="F95" s="10"/>
     </row>
     <row r="96">
-      <c r="F96" s="5"/>
+      <c r="F96" s="10"/>
     </row>
     <row r="97">
-      <c r="F97" s="5"/>
+      <c r="F97" s="10"/>
     </row>
     <row r="98">
-      <c r="F98" s="5"/>
+      <c r="F98" s="10"/>
     </row>
     <row r="99">
-      <c r="F99" s="5"/>
+      <c r="F99" s="10"/>
     </row>
     <row r="100">
-      <c r="F100" s="5"/>
+      <c r="F100" s="10"/>
     </row>
     <row r="101">
-      <c r="F101" s="5"/>
+      <c r="F101" s="10"/>
     </row>
     <row r="102">
-      <c r="F102" s="5"/>
+      <c r="F102" s="10"/>
     </row>
     <row r="103">
-      <c r="F103" s="5"/>
+      <c r="F103" s="10"/>
     </row>
     <row r="104">
-      <c r="F104" s="5"/>
+      <c r="F104" s="10"/>
     </row>
     <row r="105">
-      <c r="F105" s="5"/>
+      <c r="F105" s="10"/>
     </row>
     <row r="106">
-      <c r="F106" s="5"/>
+      <c r="F106" s="10"/>
     </row>
     <row r="107">
-      <c r="F107" s="5"/>
+      <c r="F107" s="10"/>
     </row>
     <row r="108">
-      <c r="F108" s="5"/>
+      <c r="F108" s="10"/>
     </row>
     <row r="109">
-      <c r="F109" s="5"/>
+      <c r="F109" s="10"/>
     </row>
     <row r="110">
-      <c r="F110" s="5"/>
+      <c r="F110" s="10"/>
     </row>
     <row r="111">
-      <c r="F111" s="5"/>
+      <c r="F111" s="10"/>
     </row>
     <row r="112">
-      <c r="F112" s="5"/>
+      <c r="F112" s="10"/>
     </row>
     <row r="113">
-      <c r="F113" s="5"/>
+      <c r="F113" s="10"/>
     </row>
     <row r="114">
-      <c r="F114" s="5"/>
+      <c r="F114" s="10"/>
     </row>
     <row r="115">
-      <c r="F115" s="5"/>
+      <c r="F115" s="10"/>
     </row>
     <row r="116">
-      <c r="F116" s="5"/>
+      <c r="F116" s="10"/>
     </row>
     <row r="117">
-      <c r="F117" s="5"/>
+      <c r="F117" s="10"/>
     </row>
     <row r="118">
-      <c r="F118" s="5"/>
+      <c r="F118" s="10"/>
     </row>
     <row r="119">
-      <c r="F119" s="5"/>
+      <c r="F119" s="10"/>
     </row>
     <row r="120">
-      <c r="F120" s="5"/>
+      <c r="F120" s="10"/>
     </row>
     <row r="121">
-      <c r="F121" s="5"/>
+      <c r="F121" s="10"/>
     </row>
     <row r="122">
-      <c r="F122" s="5"/>
+      <c r="F122" s="10"/>
     </row>
     <row r="123">
-      <c r="F123" s="5"/>
+      <c r="F123" s="10"/>
     </row>
     <row r="124">
-      <c r="F124" s="5"/>
+      <c r="F124" s="10"/>
     </row>
     <row r="125">
-      <c r="F125" s="5"/>
+      <c r="F125" s="10"/>
     </row>
     <row r="126">
-      <c r="F126" s="5"/>
+      <c r="F126" s="10"/>
     </row>
     <row r="127">
-      <c r="F127" s="5"/>
+      <c r="F127" s="10"/>
     </row>
     <row r="128">
-      <c r="F128" s="5"/>
+      <c r="F128" s="10"/>
     </row>
     <row r="129">
-      <c r="F129" s="5"/>
+      <c r="F129" s="10"/>
     </row>
     <row r="130">
-      <c r="F130" s="5"/>
+      <c r="F130" s="10"/>
     </row>
     <row r="131">
-      <c r="F131" s="5"/>
+      <c r="F131" s="10"/>
     </row>
     <row r="132">
-      <c r="F132" s="5"/>
+      <c r="F132" s="10"/>
     </row>
     <row r="133">
-      <c r="F133" s="5"/>
+      <c r="F133" s="10"/>
     </row>
     <row r="134">
-      <c r="F134" s="5"/>
+      <c r="F134" s="10"/>
     </row>
     <row r="135">
-      <c r="F135" s="5"/>
+      <c r="F135" s="10"/>
     </row>
     <row r="136">
-      <c r="F136" s="5"/>
+      <c r="F136" s="10"/>
     </row>
     <row r="137">
-      <c r="F137" s="5"/>
+      <c r="F137" s="10"/>
     </row>
     <row r="138">
-      <c r="F138" s="5"/>
+      <c r="F138" s="10"/>
     </row>
     <row r="139">
-      <c r="F139" s="5"/>
+      <c r="F139" s="10"/>
     </row>
     <row r="140">
-      <c r="F140" s="5"/>
+      <c r="F140" s="10"/>
     </row>
     <row r="141">
-      <c r="F141" s="5"/>
+      <c r="F141" s="10"/>
     </row>
     <row r="142">
-      <c r="F142" s="5"/>
+      <c r="F142" s="10"/>
     </row>
     <row r="143">
-      <c r="F143" s="5"/>
+      <c r="F143" s="10"/>
     </row>
     <row r="144">
-      <c r="F144" s="5"/>
+      <c r="F144" s="10"/>
     </row>
     <row r="145">
-      <c r="F145" s="5"/>
+      <c r="F145" s="10"/>
     </row>
     <row r="146">
-      <c r="F146" s="5"/>
+      <c r="F146" s="10"/>
     </row>
     <row r="147">
-      <c r="F147" s="5"/>
+      <c r="F147" s="10"/>
     </row>
     <row r="148">
-      <c r="F148" s="5"/>
+      <c r="F148" s="10"/>
     </row>
     <row r="149">
-      <c r="F149" s="5"/>
+      <c r="F149" s="10"/>
     </row>
     <row r="150">
-      <c r="F150" s="5"/>
+      <c r="F150" s="10"/>
     </row>
     <row r="151">
-      <c r="F151" s="5"/>
+      <c r="F151" s="10"/>
     </row>
     <row r="152">
-      <c r="F152" s="5"/>
+      <c r="F152" s="10"/>
     </row>
     <row r="153">
-      <c r="F153" s="5"/>
+      <c r="F153" s="10"/>
     </row>
     <row r="154">
-      <c r="F154" s="5"/>
+      <c r="F154" s="10"/>
     </row>
     <row r="155">
-      <c r="F155" s="5"/>
+      <c r="F155" s="10"/>
     </row>
     <row r="156">
-      <c r="F156" s="5"/>
+      <c r="F156" s="10"/>
     </row>
     <row r="157">
-      <c r="F157" s="5"/>
+      <c r="F157" s="10"/>
     </row>
     <row r="158">
-      <c r="F158" s="5"/>
+      <c r="F158" s="10"/>
     </row>
     <row r="159">
-      <c r="F159" s="5"/>
+      <c r="F159" s="10"/>
     </row>
     <row r="160">
-      <c r="F160" s="5"/>
+      <c r="F160" s="10"/>
     </row>
     <row r="161">
-      <c r="F161" s="5"/>
+      <c r="F161" s="10"/>
     </row>
     <row r="162">
-      <c r="F162" s="5"/>
+      <c r="F162" s="10"/>
     </row>
     <row r="163">
-      <c r="F163" s="5"/>
+      <c r="F163" s="10"/>
     </row>
     <row r="164">
-      <c r="F164" s="5"/>
+      <c r="F164" s="10"/>
     </row>
     <row r="165">
-      <c r="F165" s="5"/>
+      <c r="F165" s="10"/>
     </row>
     <row r="166">
-      <c r="F166" s="5"/>
+      <c r="F166" s="10"/>
     </row>
     <row r="167">
-      <c r="F167" s="5"/>
+      <c r="F167" s="10"/>
     </row>
     <row r="168">
-      <c r="F168" s="5"/>
+      <c r="F168" s="10"/>
     </row>
     <row r="169">
-      <c r="F169" s="5"/>
+      <c r="F169" s="10"/>
     </row>
     <row r="170">
-      <c r="F170" s="5"/>
+      <c r="F170" s="10"/>
     </row>
     <row r="171">
-      <c r="F171" s="5"/>
+      <c r="F171" s="10"/>
     </row>
     <row r="172">
-      <c r="F172" s="5"/>
+      <c r="F172" s="10"/>
     </row>
     <row r="173">
-      <c r="F173" s="5"/>
+      <c r="F173" s="10"/>
     </row>
     <row r="174">
-      <c r="F174" s="5"/>
+      <c r="F174" s="10"/>
     </row>
     <row r="175">
-      <c r="F175" s="5"/>
+      <c r="F175" s="10"/>
     </row>
     <row r="176">
-      <c r="F176" s="5"/>
+      <c r="F176" s="10"/>
     </row>
     <row r="177">
-      <c r="F177" s="5"/>
+      <c r="F177" s="10"/>
     </row>
     <row r="178">
-      <c r="F178" s="5"/>
+      <c r="F178" s="10"/>
     </row>
     <row r="179">
-      <c r="F179" s="5"/>
+      <c r="F179" s="10"/>
     </row>
     <row r="180">
-      <c r="F180" s="5"/>
+      <c r="F180" s="10"/>
     </row>
     <row r="181">
-      <c r="F181" s="5"/>
+      <c r="F181" s="10"/>
     </row>
     <row r="182">
-      <c r="F182" s="5"/>
+      <c r="F182" s="10"/>
     </row>
     <row r="183">
-      <c r="F183" s="5"/>
+      <c r="F183" s="10"/>
     </row>
     <row r="184">
-      <c r="F184" s="5"/>
+      <c r="F184" s="10"/>
     </row>
     <row r="185">
-      <c r="F185" s="5"/>
+      <c r="F185" s="10"/>
     </row>
     <row r="186">
-      <c r="F186" s="5"/>
+      <c r="F186" s="10"/>
     </row>
     <row r="187">
-      <c r="F187" s="5"/>
+      <c r="F187" s="10"/>
     </row>
     <row r="188">
-      <c r="F188" s="5"/>
+      <c r="F188" s="10"/>
     </row>
     <row r="189">
-      <c r="F189" s="5"/>
+      <c r="F189" s="10"/>
     </row>
     <row r="190">
-      <c r="F190" s="5"/>
+      <c r="F190" s="10"/>
     </row>
     <row r="191">
-      <c r="F191" s="5"/>
+      <c r="F191" s="10"/>
     </row>
     <row r="192">
-      <c r="F192" s="5"/>
+      <c r="F192" s="10"/>
     </row>
     <row r="193">
-      <c r="F193" s="5"/>
+      <c r="F193" s="10"/>
     </row>
     <row r="194">
-      <c r="F194" s="5"/>
+      <c r="F194" s="10"/>
     </row>
     <row r="195">
-      <c r="F195" s="5"/>
+      <c r="F195" s="10"/>
     </row>
     <row r="196">
-      <c r="F196" s="5"/>
+      <c r="F196" s="10"/>
     </row>
     <row r="197">
-      <c r="F197" s="5"/>
+      <c r="F197" s="10"/>
     </row>
     <row r="198">
-      <c r="F198" s="5"/>
+      <c r="F198" s="10"/>
     </row>
     <row r="199">
-      <c r="F199" s="5"/>
+      <c r="F199" s="10"/>
     </row>
     <row r="200">
-      <c r="F200" s="5"/>
+      <c r="F200" s="10"/>
     </row>
     <row r="201">
-      <c r="F201" s="5"/>
+      <c r="F201" s="10"/>
     </row>
     <row r="202">
-      <c r="F202" s="5"/>
+      <c r="F202" s="10"/>
     </row>
     <row r="203">
-      <c r="F203" s="5"/>
+      <c r="F203" s="10"/>
     </row>
     <row r="204">
-      <c r="F204" s="5"/>
+      <c r="F204" s="10"/>
     </row>
     <row r="205">
-      <c r="F205" s="5"/>
+      <c r="F205" s="10"/>
     </row>
     <row r="206">
-      <c r="F206" s="5"/>
+      <c r="F206" s="10"/>
     </row>
     <row r="207">
-      <c r="F207" s="5"/>
+      <c r="F207" s="10"/>
     </row>
     <row r="208">
-      <c r="F208" s="5"/>
+      <c r="F208" s="10"/>
     </row>
     <row r="209">
-      <c r="F209" s="5"/>
+      <c r="F209" s="10"/>
     </row>
     <row r="210">
-      <c r="F210" s="5"/>
+      <c r="F210" s="10"/>
     </row>
     <row r="211">
-      <c r="F211" s="5"/>
+      <c r="F211" s="10"/>
     </row>
     <row r="212">
-      <c r="F212" s="5"/>
+      <c r="F212" s="10"/>
     </row>
     <row r="213">
-      <c r="F213" s="5"/>
+      <c r="F213" s="10"/>
     </row>
     <row r="214">
-      <c r="F214" s="5"/>
+      <c r="F214" s="10"/>
     </row>
     <row r="215">
-      <c r="F215" s="5"/>
+      <c r="F215" s="10"/>
     </row>
     <row r="216">
-      <c r="F216" s="5"/>
+      <c r="F216" s="10"/>
     </row>
     <row r="217">
-      <c r="F217" s="5"/>
+      <c r="F217" s="10"/>
     </row>
     <row r="218">
-      <c r="F218" s="5"/>
+      <c r="F218" s="10"/>
     </row>
     <row r="219">
-      <c r="F219" s="5"/>
+      <c r="F219" s="10"/>
     </row>
     <row r="220">
-      <c r="F220" s="5"/>
+      <c r="F220" s="10"/>
     </row>
     <row r="221">
-      <c r="F221" s="5"/>
+      <c r="F221" s="10"/>
     </row>
     <row r="222">
-      <c r="F222" s="5"/>
+      <c r="F222" s="10"/>
     </row>
     <row r="223">
-      <c r="F223" s="5"/>
+      <c r="F223" s="10"/>
     </row>
     <row r="224">
-      <c r="F224" s="5"/>
+      <c r="F224" s="10"/>
     </row>
     <row r="225">
-      <c r="F225" s="5"/>
+      <c r="F225" s="10"/>
     </row>
     <row r="226">
-      <c r="F226" s="5"/>
+      <c r="F226" s="10"/>
     </row>
     <row r="227">
-      <c r="F227" s="5"/>
+      <c r="F227" s="10"/>
     </row>
     <row r="228">
-      <c r="F228" s="5"/>
+      <c r="F228" s="10"/>
     </row>
     <row r="229">
-      <c r="F229" s="5"/>
+      <c r="F229" s="10"/>
     </row>
     <row r="230">
-      <c r="F230" s="5"/>
+      <c r="F230" s="10"/>
     </row>
     <row r="231">
-      <c r="F231" s="5"/>
+      <c r="F231" s="10"/>
     </row>
     <row r="232">
-      <c r="F232" s="5"/>
+      <c r="F232" s="10"/>
     </row>
     <row r="233">
-      <c r="F233" s="5"/>
+      <c r="F233" s="10"/>
     </row>
     <row r="234">
-      <c r="F234" s="5"/>
+      <c r="F234" s="10"/>
     </row>
     <row r="235">
-      <c r="F235" s="5"/>
+      <c r="F235" s="10"/>
     </row>
     <row r="236">
-      <c r="F236" s="5"/>
+      <c r="F236" s="10"/>
     </row>
     <row r="237">
-      <c r="F237" s="5"/>
+      <c r="F237" s="10"/>
     </row>
     <row r="238">
-      <c r="F238" s="5"/>
+      <c r="F238" s="10"/>
     </row>
     <row r="239">
-      <c r="F239" s="5"/>
+      <c r="F239" s="10"/>
     </row>
     <row r="240">
-      <c r="F240" s="5"/>
+      <c r="F240" s="10"/>
     </row>
     <row r="241">
-      <c r="F241" s="5"/>
+      <c r="F241" s="10"/>
     </row>
     <row r="242">
-      <c r="F242" s="5"/>
+      <c r="F242" s="10"/>
     </row>
     <row r="243">
-      <c r="F243" s="5"/>
+      <c r="F243" s="10"/>
     </row>
     <row r="244">
-      <c r="F244" s="5"/>
+      <c r="F244" s="10"/>
     </row>
     <row r="245">
-      <c r="F245" s="5"/>
+      <c r="F245" s="10"/>
     </row>
     <row r="246">
-      <c r="F246" s="5"/>
+      <c r="F246" s="10"/>
     </row>
     <row r="247">
-      <c r="F247" s="5"/>
+      <c r="F247" s="10"/>
     </row>
     <row r="248">
-      <c r="F248" s="5"/>
+      <c r="F248" s="10"/>
     </row>
     <row r="249">
-      <c r="F249" s="5"/>
+      <c r="F249" s="10"/>
     </row>
     <row r="250">
-      <c r="F250" s="5"/>
+      <c r="F250" s="10"/>
     </row>
     <row r="251">
-      <c r="F251" s="5"/>
+      <c r="F251" s="10"/>
     </row>
     <row r="252">
-      <c r="F252" s="5"/>
+      <c r="F252" s="10"/>
     </row>
     <row r="253">
-      <c r="F253" s="5"/>
+      <c r="F253" s="10"/>
     </row>
     <row r="254">
-      <c r="F254" s="5"/>
+      <c r="F254" s="10"/>
     </row>
     <row r="255">
-      <c r="F255" s="5"/>
+      <c r="F255" s="10"/>
     </row>
     <row r="256">
-      <c r="F256" s="5"/>
+      <c r="F256" s="10"/>
     </row>
     <row r="257">
-      <c r="F257" s="5"/>
+      <c r="F257" s="10"/>
     </row>
     <row r="258">
-      <c r="F258" s="5"/>
+      <c r="F258" s="10"/>
     </row>
     <row r="259">
-      <c r="F259" s="5"/>
+      <c r="F259" s="10"/>
     </row>
     <row r="260">
-      <c r="F260" s="5"/>
+      <c r="F260" s="10"/>
     </row>
     <row r="261">
-      <c r="F261" s="5"/>
+      <c r="F261" s="10"/>
     </row>
     <row r="262">
-      <c r="F262" s="5"/>
+      <c r="F262" s="10"/>
     </row>
     <row r="263">
-      <c r="F263" s="5"/>
+      <c r="F263" s="10"/>
     </row>
     <row r="264">
-      <c r="F264" s="5"/>
+      <c r="F264" s="10"/>
     </row>
     <row r="265">
-      <c r="F265" s="5"/>
+      <c r="F265" s="10"/>
     </row>
     <row r="266">
-      <c r="F266" s="5"/>
+      <c r="F266" s="10"/>
     </row>
     <row r="267">
-      <c r="F267" s="5"/>
+      <c r="F267" s="10"/>
     </row>
     <row r="268">
-      <c r="F268" s="5"/>
+      <c r="F268" s="10"/>
     </row>
     <row r="269">
-      <c r="F269" s="5"/>
+      <c r="F269" s="10"/>
     </row>
     <row r="270">
-      <c r="F270" s="5"/>
+      <c r="F270" s="10"/>
     </row>
     <row r="271">
-      <c r="F271" s="5"/>
+      <c r="F271" s="10"/>
     </row>
     <row r="272">
-      <c r="F272" s="5"/>
+      <c r="F272" s="10"/>
     </row>
     <row r="273">
-      <c r="F273" s="5"/>
+      <c r="F273" s="10"/>
     </row>
     <row r="274">
-      <c r="F274" s="5"/>
+      <c r="F274" s="10"/>
     </row>
     <row r="275">
-      <c r="F275" s="5"/>
+      <c r="F275" s="10"/>
     </row>
     <row r="276">
-      <c r="F276" s="5"/>
+      <c r="F276" s="10"/>
     </row>
     <row r="277">
-      <c r="F277" s="5"/>
+      <c r="F277" s="10"/>
     </row>
     <row r="278">
-      <c r="F278" s="5"/>
+      <c r="F278" s="10"/>
     </row>
     <row r="279">
-      <c r="F279" s="5"/>
+      <c r="F279" s="10"/>
     </row>
     <row r="280">
-      <c r="F280" s="5"/>
+      <c r="F280" s="10"/>
     </row>
     <row r="281">
-      <c r="F281" s="5"/>
+      <c r="F281" s="10"/>
     </row>
     <row r="282">
-      <c r="F282" s="5"/>
+      <c r="F282" s="10"/>
     </row>
     <row r="283">
-      <c r="F283" s="5"/>
+      <c r="F283" s="10"/>
     </row>
     <row r="284">
-      <c r="F284" s="5"/>
+      <c r="F284" s="10"/>
     </row>
     <row r="285">
-      <c r="F285" s="5"/>
+      <c r="F285" s="10"/>
     </row>
     <row r="286">
-      <c r="F286" s="5"/>
+      <c r="F286" s="10"/>
     </row>
     <row r="287">
-      <c r="F287" s="5"/>
+      <c r="F287" s="10"/>
     </row>
     <row r="288">
-      <c r="F288" s="5"/>
+      <c r="F288" s="10"/>
     </row>
     <row r="289">
-      <c r="F289" s="5"/>
+      <c r="F289" s="10"/>
     </row>
     <row r="290">
-      <c r="F290" s="5"/>
+      <c r="F290" s="10"/>
     </row>
     <row r="291">
-      <c r="F291" s="5"/>
+      <c r="F291" s="10"/>
     </row>
     <row r="292">
-      <c r="F292" s="5"/>
+      <c r="F292" s="10"/>
     </row>
     <row r="293">
-      <c r="F293" s="5"/>
+      <c r="F293" s="10"/>
     </row>
     <row r="294">
-      <c r="F294" s="5"/>
+      <c r="F294" s="10"/>
     </row>
     <row r="295">
-      <c r="F295" s="5"/>
+      <c r="F295" s="10"/>
     </row>
     <row r="296">
-      <c r="F296" s="5"/>
+      <c r="F296" s="10"/>
     </row>
     <row r="297">
-      <c r="F297" s="5"/>
+      <c r="F297" s="10"/>
     </row>
     <row r="298">
-      <c r="F298" s="5"/>
+      <c r="F298" s="10"/>
     </row>
     <row r="299">
-      <c r="F299" s="5"/>
+      <c r="F299" s="10"/>
     </row>
     <row r="300">
-      <c r="F300" s="5"/>
+      <c r="F300" s="10"/>
     </row>
     <row r="301">
-      <c r="F301" s="5"/>
+      <c r="F301" s="10"/>
     </row>
     <row r="302">
-      <c r="F302" s="5"/>
+      <c r="F302" s="10"/>
     </row>
     <row r="303">
-      <c r="F303" s="5"/>
+      <c r="F303" s="10"/>
     </row>
     <row r="304">
-      <c r="F304" s="5"/>
+      <c r="F304" s="10"/>
     </row>
     <row r="305">
-      <c r="F305" s="5"/>
+      <c r="F305" s="10"/>
     </row>
     <row r="306">
-      <c r="F306" s="5"/>
+      <c r="F306" s="10"/>
     </row>
     <row r="307">
-      <c r="F307" s="5"/>
+      <c r="F307" s="10"/>
     </row>
     <row r="308">
-      <c r="F308" s="5"/>
+      <c r="F308" s="10"/>
     </row>
     <row r="309">
-      <c r="F309" s="5"/>
+      <c r="F309" s="10"/>
     </row>
     <row r="310">
-      <c r="F310" s="5"/>
+      <c r="F310" s="10"/>
     </row>
     <row r="311">
-      <c r="F311" s="5"/>
+      <c r="F311" s="10"/>
     </row>
     <row r="312">
-      <c r="F312" s="5"/>
+      <c r="F312" s="10"/>
     </row>
     <row r="313">
-      <c r="F313" s="5"/>
+      <c r="F313" s="10"/>
     </row>
     <row r="314">
-      <c r="F314" s="5"/>
+      <c r="F314" s="10"/>
     </row>
     <row r="315">
-      <c r="F315" s="5"/>
+      <c r="F315" s="10"/>
     </row>
     <row r="316">
-      <c r="F316" s="5"/>
+      <c r="F316" s="10"/>
     </row>
     <row r="317">
-      <c r="F317" s="5"/>
+      <c r="F317" s="10"/>
     </row>
     <row r="318">
-      <c r="F318" s="5"/>
+      <c r="F318" s="10"/>
     </row>
     <row r="319">
-      <c r="F319" s="5"/>
+      <c r="F319" s="10"/>
     </row>
     <row r="320">
-      <c r="F320" s="5"/>
+      <c r="F320" s="10"/>
     </row>
     <row r="321">
-      <c r="F321" s="5"/>
+      <c r="F321" s="10"/>
     </row>
     <row r="322">
-      <c r="F322" s="5"/>
+      <c r="F322" s="10"/>
     </row>
     <row r="323">
-      <c r="F323" s="5"/>
+      <c r="F323" s="10"/>
     </row>
     <row r="324">
-      <c r="F324" s="5"/>
+      <c r="F324" s="10"/>
     </row>
     <row r="325">
-      <c r="F325" s="5"/>
+      <c r="F325" s="10"/>
     </row>
     <row r="326">
-      <c r="F326" s="5"/>
+      <c r="F326" s="10"/>
     </row>
     <row r="327">
-      <c r="F327" s="5"/>
+      <c r="F327" s="10"/>
     </row>
     <row r="328">
-      <c r="F328" s="5"/>
+      <c r="F328" s="10"/>
     </row>
     <row r="329">
-      <c r="F329" s="5"/>
+      <c r="F329" s="10"/>
     </row>
     <row r="330">
-      <c r="F330" s="5"/>
+      <c r="F330" s="10"/>
     </row>
     <row r="331">
-      <c r="F331" s="5"/>
+      <c r="F331" s="10"/>
     </row>
     <row r="332">
-      <c r="F332" s="5"/>
+      <c r="F332" s="10"/>
     </row>
     <row r="333">
-      <c r="F333" s="5"/>
+      <c r="F333" s="10"/>
     </row>
     <row r="334">
-      <c r="F334" s="5"/>
+      <c r="F334" s="10"/>
     </row>
     <row r="335">
-      <c r="F335" s="5"/>
+      <c r="F335" s="10"/>
     </row>
     <row r="336">
-      <c r="F336" s="5"/>
+      <c r="F336" s="10"/>
     </row>
     <row r="337">
-      <c r="F337" s="5"/>
+      <c r="F337" s="10"/>
     </row>
     <row r="338">
-      <c r="F338" s="5"/>
+      <c r="F338" s="10"/>
     </row>
     <row r="339">
-      <c r="F339" s="5"/>
+      <c r="F339" s="10"/>
     </row>
     <row r="340">
-      <c r="F340" s="5"/>
+      <c r="F340" s="10"/>
     </row>
     <row r="341">
-      <c r="F341" s="5"/>
+      <c r="F341" s="10"/>
     </row>
     <row r="342">
-      <c r="F342" s="5"/>
+      <c r="F342" s="10"/>
     </row>
     <row r="343">
-      <c r="F343" s="5"/>
+      <c r="F343" s="10"/>
     </row>
     <row r="344">
-      <c r="F344" s="5"/>
+      <c r="F344" s="10"/>
     </row>
     <row r="345">
-      <c r="F345" s="5"/>
+      <c r="F345" s="10"/>
     </row>
     <row r="346">
-      <c r="F346" s="5"/>
+      <c r="F346" s="10"/>
     </row>
     <row r="347">
-      <c r="F347" s="5"/>
+      <c r="F347" s="10"/>
     </row>
     <row r="348">
-      <c r="F348" s="5"/>
+      <c r="F348" s="10"/>
     </row>
     <row r="349">
-      <c r="F349" s="5"/>
+      <c r="F349" s="10"/>
     </row>
     <row r="350">
-      <c r="F350" s="5"/>
+      <c r="F350" s="10"/>
     </row>
     <row r="351">
-      <c r="F351" s="5"/>
+      <c r="F351" s="10"/>
     </row>
     <row r="352">
-      <c r="F352" s="5"/>
+      <c r="F352" s="10"/>
     </row>
     <row r="353">
-      <c r="F353" s="5"/>
+      <c r="F353" s="10"/>
     </row>
     <row r="354">
-      <c r="F354" s="5"/>
+      <c r="F354" s="10"/>
     </row>
     <row r="355">
-      <c r="F355" s="5"/>
+      <c r="F355" s="10"/>
     </row>
     <row r="356">
-      <c r="F356" s="5"/>
+      <c r="F356" s="10"/>
     </row>
     <row r="357">
-      <c r="F357" s="5"/>
+      <c r="F357" s="10"/>
     </row>
     <row r="358">
-      <c r="F358" s="5"/>
+      <c r="F358" s="10"/>
     </row>
     <row r="359">
-      <c r="F359" s="5"/>
+      <c r="F359" s="10"/>
     </row>
     <row r="360">
-      <c r="F360" s="5"/>
+      <c r="F360" s="10"/>
     </row>
     <row r="361">
-      <c r="F361" s="5"/>
+      <c r="F361" s="10"/>
     </row>
     <row r="362">
-      <c r="F362" s="5"/>
+      <c r="F362" s="10"/>
     </row>
     <row r="363">
-      <c r="F363" s="5"/>
+      <c r="F363" s="10"/>
     </row>
     <row r="364">
-      <c r="F364" s="5"/>
+      <c r="F364" s="10"/>
     </row>
     <row r="365">
-      <c r="F365" s="5"/>
+      <c r="F365" s="10"/>
     </row>
     <row r="366">
-      <c r="F366" s="5"/>
+      <c r="F366" s="10"/>
     </row>
     <row r="367">
-      <c r="F367" s="5"/>
+      <c r="F367" s="10"/>
     </row>
     <row r="368">
-      <c r="F368" s="5"/>
+      <c r="F368" s="10"/>
     </row>
     <row r="369">
-      <c r="F369" s="5"/>
+      <c r="F369" s="10"/>
     </row>
     <row r="370">
-      <c r="F370" s="5"/>
+      <c r="F370" s="10"/>
     </row>
     <row r="371">
-      <c r="F371" s="5"/>
+      <c r="F371" s="10"/>
     </row>
     <row r="372">
-      <c r="F372" s="5"/>
+      <c r="F372" s="10"/>
     </row>
     <row r="373">
-      <c r="F373" s="5"/>
+      <c r="F373" s="10"/>
     </row>
     <row r="374">
-      <c r="F374" s="5"/>
+      <c r="F374" s="10"/>
     </row>
     <row r="375">
-      <c r="F375" s="5"/>
+      <c r="F375" s="10"/>
     </row>
     <row r="376">
-      <c r="F376" s="5"/>
+      <c r="F376" s="10"/>
     </row>
     <row r="377">
-      <c r="F377" s="5"/>
+      <c r="F377" s="10"/>
     </row>
     <row r="378">
-      <c r="F378" s="5"/>
+      <c r="F378" s="10"/>
     </row>
     <row r="379">
-      <c r="F379" s="5"/>
+      <c r="F379" s="10"/>
     </row>
     <row r="380">
-      <c r="F380" s="5"/>
+      <c r="F380" s="10"/>
     </row>
     <row r="381">
-      <c r="F381" s="5"/>
+      <c r="F381" s="10"/>
     </row>
     <row r="382">
-      <c r="F382" s="5"/>
+      <c r="F382" s="10"/>
     </row>
     <row r="383">
-      <c r="F383" s="5"/>
+      <c r="F383" s="10"/>
     </row>
     <row r="384">
-      <c r="F384" s="5"/>
+      <c r="F384" s="10"/>
     </row>
     <row r="385">
-      <c r="F385" s="5"/>
+      <c r="F385" s="10"/>
     </row>
     <row r="386">
-      <c r="F386" s="5"/>
+      <c r="F386" s="10"/>
     </row>
     <row r="387">
-      <c r="F387" s="5"/>
+      <c r="F387" s="10"/>
     </row>
     <row r="388">
-      <c r="F388" s="5"/>
+      <c r="F388" s="10"/>
     </row>
     <row r="389">
-      <c r="F389" s="5"/>
+      <c r="F389" s="10"/>
     </row>
     <row r="390">
-      <c r="F390" s="5"/>
+      <c r="F390" s="10"/>
     </row>
     <row r="391">
-      <c r="F391" s="5"/>
+      <c r="F391" s="10"/>
     </row>
     <row r="392">
-      <c r="F392" s="5"/>
+      <c r="F392" s="10"/>
     </row>
     <row r="393">
-      <c r="F393" s="5"/>
+      <c r="F393" s="10"/>
     </row>
     <row r="394">
-      <c r="F394" s="5"/>
+      <c r="F394" s="10"/>
     </row>
     <row r="395">
-      <c r="F395" s="5"/>
+      <c r="F395" s="10"/>
     </row>
     <row r="396">
-      <c r="F396" s="5"/>
+      <c r="F396" s="10"/>
     </row>
     <row r="397">
-      <c r="F397" s="5"/>
+      <c r="F397" s="10"/>
     </row>
     <row r="398">
-      <c r="F398" s="5"/>
+      <c r="F398" s="10"/>
     </row>
     <row r="399">
-      <c r="F399" s="5"/>
+      <c r="F399" s="10"/>
     </row>
     <row r="400">
-      <c r="F400" s="5"/>
+      <c r="F400" s="10"/>
     </row>
     <row r="401">
-      <c r="F401" s="5"/>
+      <c r="F401" s="10"/>
     </row>
     <row r="402">
-      <c r="F402" s="5"/>
+      <c r="F402" s="10"/>
     </row>
     <row r="403">
-      <c r="F403" s="5"/>
+      <c r="F403" s="10"/>
     </row>
     <row r="404">
-      <c r="F404" s="5"/>
+      <c r="F404" s="10"/>
     </row>
     <row r="405">
-      <c r="F405" s="5"/>
+      <c r="F405" s="10"/>
     </row>
     <row r="406">
-      <c r="F406" s="5"/>
+      <c r="F406" s="10"/>
     </row>
     <row r="407">
-      <c r="F407" s="5"/>
+      <c r="F407" s="10"/>
     </row>
     <row r="408">
-      <c r="F408" s="5"/>
+      <c r="F408" s="10"/>
     </row>
     <row r="409">
-      <c r="F409" s="5"/>
+      <c r="F409" s="10"/>
     </row>
     <row r="410">
-      <c r="F410" s="5"/>
+      <c r="F410" s="10"/>
     </row>
     <row r="411">
-      <c r="F411" s="5"/>
+      <c r="F411" s="10"/>
     </row>
     <row r="412">
-      <c r="F412" s="5"/>
+      <c r="F412" s="10"/>
     </row>
     <row r="413">
-      <c r="F413" s="5"/>
+      <c r="F413" s="10"/>
     </row>
     <row r="414">
-      <c r="F414" s="5"/>
+      <c r="F414" s="10"/>
     </row>
     <row r="415">
-      <c r="F415" s="5"/>
+      <c r="F415" s="10"/>
     </row>
     <row r="416">
-      <c r="F416" s="5"/>
+      <c r="F416" s="10"/>
     </row>
     <row r="417">
-      <c r="F417" s="5"/>
+      <c r="F417" s="10"/>
     </row>
     <row r="418">
-      <c r="F418" s="5"/>
+      <c r="F418" s="10"/>
     </row>
     <row r="419">
-      <c r="F419" s="5"/>
+      <c r="F419" s="10"/>
     </row>
     <row r="420">
-      <c r="F420" s="5"/>
+      <c r="F420" s="10"/>
     </row>
     <row r="421">
-      <c r="F421" s="5"/>
+      <c r="F421" s="10"/>
     </row>
     <row r="422">
-      <c r="F422" s="5"/>
+      <c r="F422" s="10"/>
     </row>
     <row r="423">
-      <c r="F423" s="5"/>
+      <c r="F423" s="10"/>
     </row>
     <row r="424">
-      <c r="F424" s="5"/>
+      <c r="F424" s="10"/>
     </row>
     <row r="425">
-      <c r="F425" s="5"/>
+      <c r="F425" s="10"/>
     </row>
     <row r="426">
-      <c r="F426" s="5"/>
+      <c r="F426" s="10"/>
     </row>
     <row r="427">
-      <c r="F427" s="5"/>
+      <c r="F427" s="10"/>
     </row>
     <row r="428">
-      <c r="F428" s="5"/>
+      <c r="F428" s="10"/>
     </row>
     <row r="429">
-      <c r="F429" s="5"/>
+      <c r="F429" s="10"/>
     </row>
     <row r="430">
-      <c r="F430" s="5"/>
+      <c r="F430" s="10"/>
     </row>
     <row r="431">
-      <c r="F431" s="5"/>
+      <c r="F431" s="10"/>
     </row>
     <row r="432">
-      <c r="F432" s="5"/>
+      <c r="F432" s="10"/>
     </row>
     <row r="433">
-      <c r="F433" s="5"/>
+      <c r="F433" s="10"/>
     </row>
     <row r="434">
-      <c r="F434" s="5"/>
+      <c r="F434" s="10"/>
     </row>
     <row r="435">
-      <c r="F435" s="5"/>
+      <c r="F435" s="10"/>
     </row>
     <row r="436">
-      <c r="F436" s="5"/>
+      <c r="F436" s="10"/>
     </row>
     <row r="437">
-      <c r="F437" s="5"/>
+      <c r="F437" s="10"/>
     </row>
     <row r="438">
-      <c r="F438" s="5"/>
+      <c r="F438" s="10"/>
     </row>
     <row r="439">
-      <c r="F439" s="5"/>
+      <c r="F439" s="10"/>
     </row>
     <row r="440">
-      <c r="F440" s="5"/>
+      <c r="F440" s="10"/>
     </row>
     <row r="441">
-      <c r="F441" s="5"/>
+      <c r="F441" s="10"/>
     </row>
     <row r="442">
-      <c r="F442" s="5"/>
+      <c r="F442" s="10"/>
     </row>
     <row r="443">
-      <c r="F443" s="5"/>
+      <c r="F443" s="10"/>
     </row>
     <row r="444">
-      <c r="F444" s="5"/>
+      <c r="F444" s="10"/>
     </row>
     <row r="445">
-      <c r="F445" s="5"/>
+      <c r="F445" s="10"/>
     </row>
     <row r="446">
-      <c r="F446" s="5"/>
+      <c r="F446" s="10"/>
     </row>
     <row r="447">
-      <c r="F447" s="5"/>
+      <c r="F447" s="10"/>
     </row>
     <row r="448">
-      <c r="F448" s="5"/>
+      <c r="F448" s="10"/>
     </row>
     <row r="449">
-      <c r="F449" s="5"/>
+      <c r="F449" s="10"/>
     </row>
     <row r="450">
-      <c r="F450" s="5"/>
+      <c r="F450" s="10"/>
     </row>
     <row r="451">
-      <c r="F451" s="5"/>
+      <c r="F451" s="10"/>
     </row>
     <row r="452">
-      <c r="F452" s="5"/>
+      <c r="F452" s="10"/>
     </row>
     <row r="453">
-      <c r="F453" s="5"/>
+      <c r="F453" s="10"/>
     </row>
     <row r="454">
-      <c r="F454" s="5"/>
+      <c r="F454" s="10"/>
     </row>
     <row r="455">
-      <c r="F455" s="5"/>
+      <c r="F455" s="10"/>
     </row>
     <row r="456">
-      <c r="F456" s="5"/>
+      <c r="F456" s="10"/>
     </row>
     <row r="457">
-      <c r="F457" s="5"/>
+      <c r="F457" s="10"/>
     </row>
     <row r="458">
-      <c r="F458" s="5"/>
+      <c r="F458" s="10"/>
     </row>
     <row r="459">
-      <c r="F459" s="5"/>
+      <c r="F459" s="10"/>
     </row>
     <row r="460">
-      <c r="F460" s="5"/>
+      <c r="F460" s="10"/>
     </row>
     <row r="461">
-      <c r="F461" s="5"/>
+      <c r="F461" s="10"/>
     </row>
     <row r="462">
-      <c r="F462" s="5"/>
+      <c r="F462" s="10"/>
     </row>
     <row r="463">
-      <c r="F463" s="5"/>
+      <c r="F463" s="10"/>
     </row>
     <row r="464">
-      <c r="F464" s="5"/>
+      <c r="F464" s="10"/>
     </row>
     <row r="465">
-      <c r="F465" s="5"/>
+      <c r="F465" s="10"/>
     </row>
     <row r="466">
-      <c r="F466" s="5"/>
+      <c r="F466" s="10"/>
     </row>
     <row r="467">
-      <c r="F467" s="5"/>
+      <c r="F467" s="10"/>
     </row>
     <row r="468">
-      <c r="F468" s="5"/>
+      <c r="F468" s="10"/>
     </row>
     <row r="469">
-      <c r="F469" s="5"/>
+      <c r="F469" s="10"/>
     </row>
     <row r="470">
-      <c r="F470" s="5"/>
+      <c r="F470" s="10"/>
     </row>
     <row r="471">
-      <c r="F471" s="5"/>
+      <c r="F471" s="10"/>
     </row>
     <row r="472">
-      <c r="F472" s="5"/>
+      <c r="F472" s="10"/>
     </row>
     <row r="473">
-      <c r="F473" s="5"/>
+      <c r="F473" s="10"/>
     </row>
     <row r="474">
-      <c r="F474" s="5"/>
+      <c r="F474" s="10"/>
     </row>
     <row r="475">
-      <c r="F475" s="5"/>
+      <c r="F475" s="10"/>
     </row>
     <row r="476">
-      <c r="F476" s="5"/>
+      <c r="F476" s="10"/>
     </row>
     <row r="477">
-      <c r="F477" s="5"/>
+      <c r="F477" s="10"/>
     </row>
     <row r="478">
-      <c r="F478" s="5"/>
+      <c r="F478" s="10"/>
     </row>
     <row r="479">
-      <c r="F479" s="5"/>
+      <c r="F479" s="10"/>
     </row>
     <row r="480">
-      <c r="F480" s="5"/>
+      <c r="F480" s="10"/>
     </row>
     <row r="481">
-      <c r="F481" s="5"/>
+      <c r="F481" s="10"/>
     </row>
     <row r="482">
-      <c r="F482" s="5"/>
+      <c r="F482" s="10"/>
     </row>
     <row r="483">
-      <c r="F483" s="5"/>
+      <c r="F483" s="10"/>
     </row>
     <row r="484">
-      <c r="F484" s="5"/>
+      <c r="F484" s="10"/>
     </row>
     <row r="485">
-      <c r="F485" s="5"/>
+      <c r="F485" s="10"/>
     </row>
     <row r="486">
-      <c r="F486" s="5"/>
+      <c r="F486" s="10"/>
     </row>
     <row r="487">
-      <c r="F487" s="5"/>
+      <c r="F487" s="10"/>
     </row>
     <row r="488">
-      <c r="F488" s="5"/>
+      <c r="F488" s="10"/>
     </row>
     <row r="489">
-      <c r="F489" s="5"/>
+      <c r="F489" s="10"/>
     </row>
     <row r="490">
-      <c r="F490" s="5"/>
+      <c r="F490" s="10"/>
     </row>
     <row r="491">
-      <c r="F491" s="5"/>
+      <c r="F491" s="10"/>
     </row>
     <row r="492">
-      <c r="F492" s="5"/>
+      <c r="F492" s="10"/>
     </row>
     <row r="493">
-      <c r="F493" s="5"/>
+      <c r="F493" s="10"/>
     </row>
     <row r="494">
-      <c r="F494" s="5"/>
+      <c r="F494" s="10"/>
     </row>
     <row r="495">
-      <c r="F495" s="5"/>
+      <c r="F495" s="10"/>
     </row>
     <row r="496">
-      <c r="F496" s="5"/>
+      <c r="F496" s="10"/>
     </row>
     <row r="497">
-      <c r="F497" s="5"/>
+      <c r="F497" s="10"/>
     </row>
     <row r="498">
-      <c r="F498" s="5"/>
+      <c r="F498" s="10"/>
     </row>
     <row r="499">
-      <c r="F499" s="5"/>
+      <c r="F499" s="10"/>
     </row>
     <row r="500">
-      <c r="F500" s="5"/>
+      <c r="F500" s="10"/>
     </row>
     <row r="501">
-      <c r="F501" s="5"/>
+      <c r="F501" s="10"/>
     </row>
     <row r="502">
-      <c r="F502" s="5"/>
+      <c r="F502" s="10"/>
     </row>
     <row r="503">
-      <c r="F503" s="5"/>
+      <c r="F503" s="10"/>
     </row>
     <row r="504">
-      <c r="F504" s="5"/>
+      <c r="F504" s="10"/>
     </row>
     <row r="505">
-      <c r="F505" s="5"/>
+      <c r="F505" s="10"/>
     </row>
     <row r="506">
-      <c r="F506" s="5"/>
+      <c r="F506" s="10"/>
     </row>
     <row r="507">
-      <c r="F507" s="5"/>
+      <c r="F507" s="10"/>
     </row>
     <row r="508">
-      <c r="F508" s="5"/>
+      <c r="F508" s="10"/>
     </row>
     <row r="509">
-      <c r="F509" s="5"/>
+      <c r="F509" s="10"/>
     </row>
     <row r="510">
-      <c r="F510" s="5"/>
+      <c r="F510" s="10"/>
     </row>
     <row r="511">
-      <c r="F511" s="5"/>
+      <c r="F511" s="10"/>
     </row>
     <row r="512">
-      <c r="F512" s="5"/>
+      <c r="F512" s="10"/>
     </row>
     <row r="513">
-      <c r="F513" s="5"/>
+      <c r="F513" s="10"/>
     </row>
     <row r="514">
-      <c r="F514" s="5"/>
+      <c r="F514" s="10"/>
     </row>
     <row r="515">
-      <c r="F515" s="5"/>
+      <c r="F515" s="10"/>
     </row>
     <row r="516">
-      <c r="F516" s="5"/>
+      <c r="F516" s="10"/>
     </row>
     <row r="517">
-      <c r="F517" s="5"/>
+      <c r="F517" s="10"/>
     </row>
     <row r="518">
-      <c r="F518" s="5"/>
+      <c r="F518" s="10"/>
     </row>
     <row r="519">
-      <c r="F519" s="5"/>
+      <c r="F519" s="10"/>
     </row>
     <row r="520">
-      <c r="F520" s="5"/>
+      <c r="F520" s="10"/>
     </row>
     <row r="521">
-      <c r="F521" s="5"/>
+      <c r="F521" s="10"/>
     </row>
     <row r="522">
-      <c r="F522" s="5"/>
+      <c r="F522" s="10"/>
     </row>
     <row r="523">
-      <c r="F523" s="5"/>
+      <c r="F523" s="10"/>
     </row>
     <row r="524">
-      <c r="F524" s="5"/>
+      <c r="F524" s="10"/>
     </row>
     <row r="525">
-      <c r="F525" s="5"/>
+      <c r="F525" s="10"/>
     </row>
     <row r="526">
-      <c r="F526" s="5"/>
+      <c r="F526" s="10"/>
     </row>
     <row r="527">
-      <c r="F527" s="5"/>
+      <c r="F527" s="10"/>
     </row>
     <row r="528">
-      <c r="F528" s="5"/>
+      <c r="F528" s="10"/>
     </row>
     <row r="529">
-      <c r="F529" s="5"/>
+      <c r="F529" s="10"/>
     </row>
     <row r="530">
-      <c r="F530" s="5"/>
+      <c r="F530" s="10"/>
     </row>
     <row r="531">
-      <c r="F531" s="5"/>
+      <c r="F531" s="10"/>
     </row>
     <row r="532">
-      <c r="F532" s="5"/>
+      <c r="F532" s="10"/>
     </row>
     <row r="533">
-      <c r="F533" s="5"/>
+      <c r="F533" s="10"/>
     </row>
     <row r="534">
-      <c r="F534" s="5"/>
+      <c r="F534" s="10"/>
     </row>
     <row r="535">
-      <c r="F535" s="5"/>
+      <c r="F535" s="10"/>
     </row>
     <row r="536">
-      <c r="F536" s="5"/>
+      <c r="F536" s="10"/>
     </row>
     <row r="537">
-      <c r="F537" s="5"/>
+      <c r="F537" s="10"/>
     </row>
     <row r="538">
-      <c r="F538" s="5"/>
+      <c r="F538" s="10"/>
     </row>
     <row r="539">
-      <c r="F539" s="5"/>
+      <c r="F539" s="10"/>
     </row>
     <row r="540">
-      <c r="F540" s="5"/>
+      <c r="F540" s="10"/>
     </row>
     <row r="541">
-      <c r="F541" s="5"/>
+      <c r="F541" s="10"/>
     </row>
     <row r="542">
-      <c r="F542" s="5"/>
+      <c r="F542" s="10"/>
     </row>
     <row r="543">
-      <c r="F543" s="5"/>
+      <c r="F543" s="10"/>
     </row>
     <row r="544">
-      <c r="F544" s="5"/>
+      <c r="F544" s="10"/>
     </row>
     <row r="545">
-      <c r="F545" s="5"/>
+      <c r="F545" s="10"/>
     </row>
     <row r="546">
-      <c r="F546" s="5"/>
+      <c r="F546" s="10"/>
     </row>
     <row r="547">
-      <c r="F547" s="5"/>
+      <c r="F547" s="10"/>
     </row>
     <row r="548">
-      <c r="F548" s="5"/>
+      <c r="F548" s="10"/>
     </row>
     <row r="549">
-      <c r="F549" s="5"/>
+      <c r="F549" s="10"/>
     </row>
     <row r="550">
-      <c r="F550" s="5"/>
+      <c r="F550" s="10"/>
     </row>
     <row r="551">
-      <c r="F551" s="5"/>
+      <c r="F551" s="10"/>
     </row>
     <row r="552">
-      <c r="F552" s="5"/>
+      <c r="F552" s="10"/>
     </row>
     <row r="553">
-      <c r="F553" s="5"/>
+      <c r="F553" s="10"/>
     </row>
     <row r="554">
-      <c r="F554" s="5"/>
+      <c r="F554" s="10"/>
     </row>
     <row r="555">
-      <c r="F555" s="5"/>
+      <c r="F555" s="10"/>
     </row>
     <row r="556">
-      <c r="F556" s="5"/>
+      <c r="F556" s="10"/>
     </row>
     <row r="557">
-      <c r="F557" s="5"/>
+      <c r="F557" s="10"/>
     </row>
     <row r="558">
-      <c r="F558" s="5"/>
+      <c r="F558" s="10"/>
     </row>
     <row r="559">
-      <c r="F559" s="5"/>
+      <c r="F559" s="10"/>
     </row>
     <row r="560">
-      <c r="F560" s="5"/>
+      <c r="F560" s="10"/>
     </row>
     <row r="561">
-      <c r="F561" s="5"/>
+      <c r="F561" s="10"/>
     </row>
     <row r="562">
-      <c r="F562" s="5"/>
+      <c r="F562" s="10"/>
     </row>
     <row r="563">
-      <c r="F563" s="5"/>
+      <c r="F563" s="10"/>
     </row>
     <row r="564">
-      <c r="F564" s="5"/>
+      <c r="F564" s="10"/>
     </row>
     <row r="565">
-      <c r="F565" s="5"/>
+      <c r="F565" s="10"/>
     </row>
     <row r="566">
-      <c r="F566" s="5"/>
+      <c r="F566" s="10"/>
     </row>
     <row r="567">
-      <c r="F567" s="5"/>
+      <c r="F567" s="10"/>
     </row>
     <row r="568">
-      <c r="F568" s="5"/>
+      <c r="F568" s="10"/>
     </row>
     <row r="569">
-      <c r="F569" s="5"/>
+      <c r="F569" s="10"/>
     </row>
     <row r="570">
-      <c r="F570" s="5"/>
+      <c r="F570" s="10"/>
     </row>
     <row r="571">
-      <c r="F571" s="5"/>
+      <c r="F571" s="10"/>
     </row>
     <row r="572">
-      <c r="F572" s="5"/>
+      <c r="F572" s="10"/>
     </row>
     <row r="573">
-      <c r="F573" s="5"/>
+      <c r="F573" s="10"/>
     </row>
     <row r="574">
-      <c r="F574" s="5"/>
+      <c r="F574" s="10"/>
     </row>
     <row r="575">
-      <c r="F575" s="5"/>
+      <c r="F575" s="10"/>
     </row>
     <row r="576">
-      <c r="F576" s="5"/>
+      <c r="F576" s="10"/>
     </row>
     <row r="577">
-      <c r="F577" s="5"/>
+      <c r="F577" s="10"/>
     </row>
     <row r="578">
-      <c r="F578" s="5"/>
+      <c r="F578" s="10"/>
     </row>
     <row r="579">
-      <c r="F579" s="5"/>
+      <c r="F579" s="10"/>
     </row>
     <row r="580">
-      <c r="F580" s="5"/>
+      <c r="F580" s="10"/>
     </row>
     <row r="581">
-      <c r="F581" s="5"/>
+      <c r="F581" s="10"/>
     </row>
     <row r="582">
-      <c r="F582" s="5"/>
+      <c r="F582" s="10"/>
     </row>
     <row r="583">
-      <c r="F583" s="5"/>
+      <c r="F583" s="10"/>
     </row>
     <row r="584">
-      <c r="F584" s="5"/>
+      <c r="F584" s="10"/>
     </row>
     <row r="585">
-      <c r="F585" s="5"/>
+      <c r="F585" s="10"/>
     </row>
     <row r="586">
-      <c r="F586" s="5"/>
+      <c r="F586" s="10"/>
     </row>
     <row r="587">
-      <c r="F587" s="5"/>
+      <c r="F587" s="10"/>
     </row>
     <row r="588">
-      <c r="F588" s="5"/>
+      <c r="F588" s="10"/>
     </row>
     <row r="589">
-      <c r="F589" s="5"/>
+      <c r="F589" s="10"/>
     </row>
     <row r="590">
-      <c r="F590" s="5"/>
+      <c r="F590" s="10"/>
     </row>
     <row r="591">
-      <c r="F591" s="5"/>
+      <c r="F591" s="10"/>
     </row>
     <row r="592">
-      <c r="F592" s="5"/>
+      <c r="F592" s="10"/>
     </row>
     <row r="593">
-      <c r="F593" s="5"/>
+      <c r="F593" s="10"/>
     </row>
     <row r="594">
-      <c r="F594" s="5"/>
+      <c r="F594" s="10"/>
     </row>
     <row r="595">
-      <c r="F595" s="5"/>
+      <c r="F595" s="10"/>
     </row>
     <row r="596">
-      <c r="F596" s="5"/>
+      <c r="F596" s="10"/>
     </row>
     <row r="597">
-      <c r="F597" s="5"/>
+      <c r="F597" s="10"/>
     </row>
     <row r="598">
-      <c r="F598" s="5"/>
+      <c r="F598" s="10"/>
     </row>
     <row r="599">
-      <c r="F599" s="5"/>
+      <c r="F599" s="10"/>
     </row>
     <row r="600">
-      <c r="F600" s="5"/>
+      <c r="F600" s="10"/>
     </row>
     <row r="601">
-      <c r="F601" s="5"/>
+      <c r="F601" s="10"/>
     </row>
     <row r="602">
-      <c r="F602" s="5"/>
+      <c r="F602" s="10"/>
     </row>
     <row r="603">
-      <c r="F603" s="5"/>
+      <c r="F603" s="10"/>
     </row>
     <row r="604">
-      <c r="F604" s="5"/>
+      <c r="F604" s="10"/>
     </row>
     <row r="605">
-      <c r="F605" s="5"/>
+      <c r="F605" s="10"/>
     </row>
     <row r="606">
-      <c r="F606" s="5"/>
+      <c r="F606" s="10"/>
     </row>
     <row r="607">
-      <c r="F607" s="5"/>
+      <c r="F607" s="10"/>
     </row>
     <row r="608">
-      <c r="F608" s="5"/>
+      <c r="F608" s="10"/>
     </row>
     <row r="609">
-      <c r="F609" s="5"/>
+      <c r="F609" s="10"/>
     </row>
     <row r="610">
-      <c r="F610" s="5"/>
+      <c r="F610" s="10"/>
     </row>
     <row r="611">
-      <c r="F611" s="5"/>
+      <c r="F611" s="10"/>
     </row>
     <row r="612">
-      <c r="F612" s="5"/>
+      <c r="F612" s="10"/>
     </row>
     <row r="613">
-      <c r="F613" s="5"/>
+      <c r="F613" s="10"/>
     </row>
     <row r="614">
-      <c r="F614" s="5"/>
+      <c r="F614" s="10"/>
     </row>
     <row r="615">
-      <c r="F615" s="5"/>
+      <c r="F615" s="10"/>
     </row>
     <row r="616">
-      <c r="F616" s="5"/>
+      <c r="F616" s="10"/>
     </row>
     <row r="617">
-      <c r="F617" s="5"/>
+      <c r="F617" s="10"/>
     </row>
     <row r="618">
-      <c r="F618" s="5"/>
+      <c r="F618" s="10"/>
     </row>
     <row r="619">
-      <c r="F619" s="5"/>
+      <c r="F619" s="10"/>
     </row>
     <row r="620">
-      <c r="F620" s="5"/>
+      <c r="F620" s="10"/>
     </row>
     <row r="621">
-      <c r="F621" s="5"/>
+      <c r="F621" s="10"/>
     </row>
     <row r="622">
-      <c r="F622" s="5"/>
+      <c r="F622" s="10"/>
     </row>
     <row r="623">
-      <c r="F623" s="5"/>
+      <c r="F623" s="10"/>
     </row>
     <row r="624">
-      <c r="F624" s="5"/>
+      <c r="F624" s="10"/>
     </row>
     <row r="625">
-      <c r="F625" s="5"/>
+      <c r="F625" s="10"/>
     </row>
     <row r="626">
-      <c r="F626" s="5"/>
+      <c r="F626" s="10"/>
     </row>
     <row r="627">
-      <c r="F627" s="5"/>
+      <c r="F627" s="10"/>
     </row>
     <row r="628">
-      <c r="F628" s="5"/>
+      <c r="F628" s="10"/>
     </row>
     <row r="629">
-      <c r="F629" s="5"/>
+      <c r="F629" s="10"/>
     </row>
     <row r="630">
-      <c r="F630" s="5"/>
+      <c r="F630" s="10"/>
     </row>
     <row r="631">
-      <c r="F631" s="5"/>
+      <c r="F631" s="10"/>
     </row>
     <row r="632">
-      <c r="F632" s="5"/>
+      <c r="F632" s="10"/>
     </row>
     <row r="633">
-      <c r="F633" s="5"/>
+      <c r="F633" s="10"/>
     </row>
     <row r="634">
-      <c r="F634" s="5"/>
+      <c r="F634" s="10"/>
     </row>
     <row r="635">
-      <c r="F635" s="5"/>
+      <c r="F635" s="10"/>
     </row>
     <row r="636">
-      <c r="F636" s="5"/>
+      <c r="F636" s="10"/>
     </row>
     <row r="637">
-      <c r="F637" s="5"/>
+      <c r="F637" s="10"/>
     </row>
     <row r="638">
-      <c r="F638" s="5"/>
+      <c r="F638" s="10"/>
     </row>
     <row r="639">
-      <c r="F639" s="5"/>
+      <c r="F639" s="10"/>
     </row>
     <row r="640">
-      <c r="F640" s="5"/>
+      <c r="F640" s="10"/>
     </row>
     <row r="641">
-      <c r="F641" s="5"/>
+      <c r="F641" s="10"/>
     </row>
     <row r="642">
-      <c r="F642" s="5"/>
+      <c r="F642" s="10"/>
     </row>
     <row r="643">
-      <c r="F643" s="5"/>
+      <c r="F643" s="10"/>
     </row>
     <row r="644">
-      <c r="F644" s="5"/>
+      <c r="F644" s="10"/>
     </row>
     <row r="645">
-      <c r="F645" s="5"/>
+      <c r="F645" s="10"/>
     </row>
     <row r="646">
-      <c r="F646" s="5"/>
+      <c r="F646" s="10"/>
     </row>
     <row r="647">
-      <c r="F647" s="5"/>
+      <c r="F647" s="10"/>
     </row>
     <row r="648">
-      <c r="F648" s="5"/>
+      <c r="F648" s="10"/>
     </row>
     <row r="649">
-      <c r="F649" s="5"/>
+      <c r="F649" s="10"/>
     </row>
     <row r="650">
-      <c r="F650" s="5"/>
+      <c r="F650" s="10"/>
     </row>
     <row r="651">
-      <c r="F651" s="5"/>
+      <c r="F651" s="10"/>
     </row>
     <row r="652">
-      <c r="F652" s="5"/>
+      <c r="F652" s="10"/>
     </row>
     <row r="653">
-      <c r="F653" s="5"/>
+      <c r="F653" s="10"/>
     </row>
     <row r="654">
-      <c r="F654" s="5"/>
+      <c r="F654" s="10"/>
     </row>
     <row r="655">
-      <c r="F655" s="5"/>
+      <c r="F655" s="10"/>
     </row>
     <row r="656">
-      <c r="F656" s="5"/>
+      <c r="F656" s="10"/>
     </row>
     <row r="657">
-      <c r="F657" s="5"/>
+      <c r="F657" s="10"/>
     </row>
     <row r="658">
-      <c r="F658" s="5"/>
+      <c r="F658" s="10"/>
     </row>
     <row r="659">
-      <c r="F659" s="5"/>
+      <c r="F659" s="10"/>
     </row>
     <row r="660">
-      <c r="F660" s="5"/>
+      <c r="F660" s="10"/>
     </row>
     <row r="661">
-      <c r="F661" s="5"/>
+      <c r="F661" s="10"/>
     </row>
     <row r="662">
-      <c r="F662" s="5"/>
+      <c r="F662" s="10"/>
     </row>
     <row r="663">
-      <c r="F663" s="5"/>
+      <c r="F663" s="10"/>
     </row>
     <row r="664">
-      <c r="F664" s="5"/>
+      <c r="F664" s="10"/>
     </row>
     <row r="665">
-      <c r="F665" s="5"/>
+      <c r="F665" s="10"/>
     </row>
     <row r="666">
-      <c r="F666" s="5"/>
+      <c r="F666" s="10"/>
     </row>
     <row r="667">
-      <c r="F667" s="5"/>
+      <c r="F667" s="10"/>
     </row>
     <row r="668">
-      <c r="F668" s="5"/>
+      <c r="F668" s="10"/>
     </row>
     <row r="669">
-      <c r="F669" s="5"/>
+      <c r="F669" s="10"/>
     </row>
     <row r="670">
-      <c r="F670" s="5"/>
+      <c r="F670" s="10"/>
     </row>
     <row r="671">
-      <c r="F671" s="5"/>
+      <c r="F671" s="10"/>
     </row>
     <row r="672">
-      <c r="F672" s="5"/>
+      <c r="F672" s="10"/>
     </row>
     <row r="673">
-      <c r="F673" s="5"/>
+      <c r="F673" s="10"/>
     </row>
     <row r="674">
-      <c r="F674" s="5"/>
+      <c r="F674" s="10"/>
     </row>
     <row r="675">
-      <c r="F675" s="5"/>
+      <c r="F675" s="10"/>
     </row>
     <row r="676">
-      <c r="F676" s="5"/>
+      <c r="F676" s="10"/>
     </row>
     <row r="677">
-      <c r="F677" s="5"/>
+      <c r="F677" s="10"/>
     </row>
     <row r="678">
-      <c r="F678" s="5"/>
+      <c r="F678" s="10"/>
     </row>
     <row r="679">
-      <c r="F679" s="5"/>
+      <c r="F679" s="10"/>
     </row>
     <row r="680">
-      <c r="F680" s="5"/>
+      <c r="F680" s="10"/>
     </row>
     <row r="681">
-      <c r="F681" s="5"/>
+      <c r="F681" s="10"/>
     </row>
     <row r="682">
-      <c r="F682" s="5"/>
+      <c r="F682" s="10"/>
     </row>
     <row r="683">
-      <c r="F683" s="5"/>
+      <c r="F683" s="10"/>
     </row>
     <row r="684">
-      <c r="F684" s="5"/>
+      <c r="F684" s="10"/>
     </row>
     <row r="685">
-      <c r="F685" s="5"/>
+      <c r="F685" s="10"/>
     </row>
     <row r="686">
-      <c r="F686" s="5"/>
+      <c r="F686" s="10"/>
     </row>
     <row r="687">
-      <c r="F687" s="5"/>
+      <c r="F687" s="10"/>
     </row>
     <row r="688">
-      <c r="F688" s="5"/>
+      <c r="F688" s="10"/>
     </row>
     <row r="689">
-      <c r="F689" s="5"/>
+      <c r="F689" s="10"/>
     </row>
     <row r="690">
-      <c r="F690" s="5"/>
+      <c r="F690" s="10"/>
     </row>
     <row r="691">
-      <c r="F691" s="5"/>
+      <c r="F691" s="10"/>
     </row>
     <row r="692">
-      <c r="F692" s="5"/>
+      <c r="F692" s="10"/>
     </row>
     <row r="693">
-      <c r="F693" s="5"/>
+      <c r="F693" s="10"/>
     </row>
     <row r="694">
-      <c r="F694" s="5"/>
+      <c r="F694" s="10"/>
     </row>
     <row r="695">
-      <c r="F695" s="5"/>
+      <c r="F695" s="10"/>
     </row>
     <row r="696">
-      <c r="F696" s="5"/>
+      <c r="F696" s="10"/>
     </row>
     <row r="697">
-      <c r="F697" s="5"/>
+      <c r="F697" s="10"/>
     </row>
     <row r="698">
-      <c r="F698" s="5"/>
+      <c r="F698" s="10"/>
     </row>
     <row r="699">
-      <c r="F699" s="5"/>
+      <c r="F699" s="10"/>
     </row>
     <row r="700">
-      <c r="F700" s="5"/>
+      <c r="F700" s="10"/>
     </row>
     <row r="701">
-      <c r="F701" s="5"/>
+      <c r="F701" s="10"/>
     </row>
     <row r="702">
-      <c r="F702" s="5"/>
+      <c r="F702" s="10"/>
     </row>
     <row r="703">
-      <c r="F703" s="5"/>
+      <c r="F703" s="10"/>
     </row>
     <row r="704">
-      <c r="F704" s="5"/>
+      <c r="F704" s="10"/>
     </row>
     <row r="705">
-      <c r="F705" s="5"/>
+      <c r="F705" s="10"/>
     </row>
     <row r="706">
-      <c r="F706" s="5"/>
+      <c r="F706" s="10"/>
     </row>
     <row r="707">
-      <c r="F707" s="5"/>
+      <c r="F707" s="10"/>
     </row>
     <row r="708">
-      <c r="F708" s="5"/>
+      <c r="F708" s="10"/>
     </row>
     <row r="709">
-      <c r="F709" s="5"/>
+      <c r="F709" s="10"/>
     </row>
     <row r="710">
-      <c r="F710" s="5"/>
+      <c r="F710" s="10"/>
     </row>
     <row r="711">
-      <c r="F711" s="5"/>
+      <c r="F711" s="10"/>
     </row>
     <row r="712">
-      <c r="F712" s="5"/>
+      <c r="F712" s="10"/>
     </row>
     <row r="713">
-      <c r="F713" s="5"/>
+      <c r="F713" s="10"/>
     </row>
     <row r="714">
-      <c r="F714" s="5"/>
+      <c r="F714" s="10"/>
     </row>
     <row r="715">
-      <c r="F715" s="5"/>
+      <c r="F715" s="10"/>
     </row>
     <row r="716">
-      <c r="F716" s="5"/>
+      <c r="F716" s="10"/>
     </row>
     <row r="717">
-      <c r="F717" s="5"/>
+      <c r="F717" s="10"/>
     </row>
     <row r="718">
-      <c r="F718" s="5"/>
+      <c r="F718" s="10"/>
     </row>
     <row r="719">
-      <c r="F719" s="5"/>
+      <c r="F719" s="10"/>
     </row>
     <row r="720">
-      <c r="F720" s="5"/>
+      <c r="F720" s="10"/>
     </row>
     <row r="721">
-      <c r="F721" s="5"/>
+      <c r="F721" s="10"/>
     </row>
     <row r="722">
-      <c r="F722" s="5"/>
+      <c r="F722" s="10"/>
     </row>
     <row r="723">
-      <c r="F723" s="5"/>
+      <c r="F723" s="10"/>
     </row>
     <row r="724">
-      <c r="F724" s="5"/>
+      <c r="F724" s="10"/>
     </row>
     <row r="725">
-      <c r="F725" s="5"/>
+      <c r="F725" s="10"/>
     </row>
     <row r="726">
-      <c r="F726" s="5"/>
+      <c r="F726" s="10"/>
     </row>
     <row r="727">
-      <c r="F727" s="5"/>
+      <c r="F727" s="10"/>
     </row>
     <row r="728">
-      <c r="F728" s="5"/>
+      <c r="F728" s="10"/>
     </row>
     <row r="729">
-      <c r="F729" s="5"/>
+      <c r="F729" s="10"/>
     </row>
     <row r="730">
-      <c r="F730" s="5"/>
+      <c r="F730" s="10"/>
     </row>
     <row r="731">
-      <c r="F731" s="5"/>
+      <c r="F731" s="10"/>
     </row>
     <row r="732">
-      <c r="F732" s="5"/>
+      <c r="F732" s="10"/>
     </row>
     <row r="733">
-      <c r="F733" s="5"/>
+      <c r="F733" s="10"/>
     </row>
     <row r="734">
-      <c r="F734" s="5"/>
+      <c r="F734" s="10"/>
     </row>
     <row r="735">
-      <c r="F735" s="5"/>
+      <c r="F735" s="10"/>
     </row>
     <row r="736">
-      <c r="F736" s="5"/>
+      <c r="F736" s="10"/>
     </row>
     <row r="737">
-      <c r="F737" s="5"/>
+      <c r="F737" s="10"/>
     </row>
     <row r="738">
-      <c r="F738" s="5"/>
+      <c r="F738" s="10"/>
     </row>
     <row r="739">
-      <c r="F739" s="5"/>
+      <c r="F739" s="10"/>
     </row>
     <row r="740">
-      <c r="F740" s="5"/>
+      <c r="F740" s="10"/>
     </row>
     <row r="741">
-      <c r="F741" s="5"/>
+      <c r="F741" s="10"/>
     </row>
     <row r="742">
-      <c r="F742" s="5"/>
+      <c r="F742" s="10"/>
     </row>
     <row r="743">
-      <c r="F743" s="5"/>
+      <c r="F743" s="10"/>
     </row>
     <row r="744">
-      <c r="F744" s="5"/>
+      <c r="F744" s="10"/>
     </row>
     <row r="745">
-      <c r="F745" s="5"/>
+      <c r="F745" s="10"/>
     </row>
     <row r="746">
-      <c r="F746" s="5"/>
+      <c r="F746" s="10"/>
     </row>
     <row r="747">
-      <c r="F747" s="5"/>
+      <c r="F747" s="10"/>
     </row>
     <row r="748">
-      <c r="F748" s="5"/>
+      <c r="F748" s="10"/>
     </row>
     <row r="749">
-      <c r="F749" s="5"/>
+      <c r="F749" s="10"/>
     </row>
     <row r="750">
-      <c r="F750" s="5"/>
+      <c r="F750" s="10"/>
     </row>
     <row r="751">
-      <c r="F751" s="5"/>
+      <c r="F751" s="10"/>
     </row>
     <row r="752">
-      <c r="F752" s="5"/>
+      <c r="F752" s="10"/>
     </row>
     <row r="753">
-      <c r="F753" s="5"/>
+      <c r="F753" s="10"/>
     </row>
     <row r="754">
-      <c r="F754" s="5"/>
+      <c r="F754" s="10"/>
     </row>
     <row r="755">
-      <c r="F755" s="5"/>
+      <c r="F755" s="10"/>
     </row>
     <row r="756">
-      <c r="F756" s="5"/>
+      <c r="F756" s="10"/>
     </row>
     <row r="757">
-      <c r="F757" s="5"/>
+      <c r="F757" s="10"/>
     </row>
     <row r="758">
-      <c r="F758" s="5"/>
+      <c r="F758" s="10"/>
     </row>
     <row r="759">
-      <c r="F759" s="5"/>
+      <c r="F759" s="10"/>
     </row>
     <row r="760">
-      <c r="F760" s="5"/>
+      <c r="F760" s="10"/>
     </row>
     <row r="761">
-      <c r="F761" s="5"/>
+      <c r="F761" s="10"/>
     </row>
     <row r="762">
-      <c r="F762" s="5"/>
+      <c r="F762" s="10"/>
     </row>
     <row r="763">
-      <c r="F763" s="5"/>
+      <c r="F763" s="10"/>
     </row>
     <row r="764">
-      <c r="F764" s="5"/>
+      <c r="F764" s="10"/>
     </row>
     <row r="765">
-      <c r="F765" s="5"/>
+      <c r="F765" s="10"/>
     </row>
     <row r="766">
-      <c r="F766" s="5"/>
+      <c r="F766" s="10"/>
     </row>
     <row r="767">
-      <c r="F767" s="5"/>
+      <c r="F767" s="10"/>
     </row>
     <row r="768">
-      <c r="F768" s="5"/>
+      <c r="F768" s="10"/>
     </row>
     <row r="769">
-      <c r="F769" s="5"/>
+      <c r="F769" s="10"/>
     </row>
     <row r="770">
-      <c r="F770" s="5"/>
+      <c r="F770" s="10"/>
     </row>
     <row r="771">
-      <c r="F771" s="5"/>
+      <c r="F771" s="10"/>
     </row>
     <row r="772">
-      <c r="F772" s="5"/>
+      <c r="F772" s="10"/>
     </row>
     <row r="773">
-      <c r="F773" s="5"/>
+      <c r="F773" s="10"/>
     </row>
     <row r="774">
-      <c r="F774" s="5"/>
+      <c r="F774" s="10"/>
     </row>
     <row r="775">
-      <c r="F775" s="5"/>
+      <c r="F775" s="10"/>
     </row>
     <row r="776">
-      <c r="F776" s="5"/>
+      <c r="F776" s="10"/>
     </row>
     <row r="777">
-      <c r="F777" s="5"/>
+      <c r="F777" s="10"/>
     </row>
     <row r="778">
-      <c r="F778" s="5"/>
+      <c r="F778" s="10"/>
     </row>
     <row r="779">
-      <c r="F779" s="5"/>
+      <c r="F779" s="10"/>
     </row>
     <row r="780">
-      <c r="F780" s="5"/>
+      <c r="F780" s="10"/>
     </row>
     <row r="781">
-      <c r="F781" s="5"/>
+      <c r="F781" s="10"/>
     </row>
     <row r="782">
-      <c r="F782" s="5"/>
+      <c r="F782" s="10"/>
     </row>
     <row r="783">
-      <c r="F783" s="5"/>
+      <c r="F783" s="10"/>
     </row>
     <row r="784">
-      <c r="F784" s="5"/>
+      <c r="F784" s="10"/>
     </row>
     <row r="785">
-      <c r="F785" s="5"/>
+      <c r="F785" s="10"/>
     </row>
     <row r="786">
-      <c r="F786" s="5"/>
+      <c r="F786" s="10"/>
     </row>
     <row r="787">
-      <c r="F787" s="5"/>
+      <c r="F787" s="10"/>
     </row>
     <row r="788">
-      <c r="F788" s="5"/>
+      <c r="F788" s="10"/>
     </row>
     <row r="789">
-      <c r="F789" s="5"/>
+      <c r="F789" s="10"/>
     </row>
     <row r="790">
-      <c r="F790" s="5"/>
+      <c r="F790" s="10"/>
     </row>
     <row r="791">
-      <c r="F791" s="5"/>
+      <c r="F791" s="10"/>
     </row>
     <row r="792">
-      <c r="F792" s="5"/>
+      <c r="F792" s="10"/>
     </row>
     <row r="793">
-      <c r="F793" s="5"/>
+      <c r="F793" s="10"/>
     </row>
     <row r="794">
-      <c r="F794" s="5"/>
+      <c r="F794" s="10"/>
     </row>
     <row r="795">
-      <c r="F795" s="5"/>
+      <c r="F795" s="10"/>
     </row>
     <row r="796">
-      <c r="F796" s="5"/>
+      <c r="F796" s="10"/>
     </row>
     <row r="797">
-      <c r="F797" s="5"/>
+      <c r="F797" s="10"/>
     </row>
     <row r="798">
-      <c r="F798" s="5"/>
+      <c r="F798" s="10"/>
     </row>
     <row r="799">
-      <c r="F799" s="5"/>
+      <c r="F799" s="10"/>
     </row>
     <row r="800">
-      <c r="F800" s="5"/>
+      <c r="F800" s="10"/>
     </row>
     <row r="801">
-      <c r="F801" s="5"/>
+      <c r="F801" s="10"/>
     </row>
     <row r="802">
-      <c r="F802" s="5"/>
+      <c r="F802" s="10"/>
     </row>
     <row r="803">
-      <c r="F803" s="5"/>
+      <c r="F803" s="10"/>
     </row>
     <row r="804">
-      <c r="F804" s="5"/>
+      <c r="F804" s="10"/>
     </row>
     <row r="805">
-      <c r="F805" s="5"/>
+      <c r="F805" s="10"/>
     </row>
     <row r="806">
-      <c r="F806" s="5"/>
+      <c r="F806" s="10"/>
     </row>
     <row r="807">
-      <c r="F807" s="5"/>
+      <c r="F807" s="10"/>
     </row>
     <row r="808">
-      <c r="F808" s="5"/>
+      <c r="F808" s="10"/>
     </row>
     <row r="809">
-      <c r="F809" s="5"/>
+      <c r="F809" s="10"/>
     </row>
     <row r="810">
-      <c r="F810" s="5"/>
+      <c r="F810" s="10"/>
     </row>
     <row r="811">
-      <c r="F811" s="5"/>
+      <c r="F811" s="10"/>
     </row>
     <row r="812">
-      <c r="F812" s="5"/>
+      <c r="F812" s="10"/>
     </row>
     <row r="813">
-      <c r="F813" s="5"/>
+      <c r="F813" s="10"/>
     </row>
     <row r="814">
-      <c r="F814" s="5"/>
+      <c r="F814" s="10"/>
     </row>
     <row r="815">
-      <c r="F815" s="5"/>
+      <c r="F815" s="10"/>
     </row>
     <row r="816">
-      <c r="F816" s="5"/>
+      <c r="F816" s="10"/>
     </row>
     <row r="817">
-      <c r="F817" s="5"/>
+      <c r="F817" s="10"/>
     </row>
     <row r="818">
-      <c r="F818" s="5"/>
+      <c r="F818" s="10"/>
     </row>
     <row r="819">
-      <c r="F819" s="5"/>
+      <c r="F819" s="10"/>
     </row>
     <row r="820">
-      <c r="F820" s="5"/>
+      <c r="F820" s="10"/>
     </row>
     <row r="821">
-      <c r="F821" s="5"/>
+      <c r="F821" s="10"/>
     </row>
     <row r="822">
-      <c r="F822" s="5"/>
+      <c r="F822" s="10"/>
     </row>
     <row r="823">
-      <c r="F823" s="5"/>
+      <c r="F823" s="10"/>
     </row>
     <row r="824">
-      <c r="F824" s="5"/>
+      <c r="F824" s="10"/>
     </row>
     <row r="825">
-      <c r="F825" s="5"/>
+      <c r="F825" s="10"/>
     </row>
     <row r="826">
-      <c r="F826" s="5"/>
+      <c r="F826" s="10"/>
     </row>
     <row r="827">
-      <c r="F827" s="5"/>
+      <c r="F827" s="10"/>
     </row>
     <row r="828">
-      <c r="F828" s="5"/>
+      <c r="F828" s="10"/>
     </row>
     <row r="829">
-      <c r="F829" s="5"/>
+      <c r="F829" s="10"/>
     </row>
     <row r="830">
-      <c r="F830" s="5"/>
+      <c r="F830" s="10"/>
     </row>
     <row r="831">
-      <c r="F831" s="5"/>
+      <c r="F831" s="10"/>
     </row>
     <row r="832">
-      <c r="F832" s="5"/>
+      <c r="F832" s="10"/>
     </row>
     <row r="833">
-      <c r="F833" s="5"/>
+      <c r="F833" s="10"/>
     </row>
     <row r="834">
-      <c r="F834" s="5"/>
+      <c r="F834" s="10"/>
     </row>
     <row r="835">
-      <c r="F835" s="5"/>
+      <c r="F835" s="10"/>
     </row>
     <row r="836">
-      <c r="F836" s="5"/>
+      <c r="F836" s="10"/>
     </row>
     <row r="837">
-      <c r="F837" s="5"/>
+      <c r="F837" s="10"/>
     </row>
     <row r="838">
-      <c r="F838" s="5"/>
+      <c r="F838" s="10"/>
     </row>
     <row r="839">
-      <c r="F839" s="5"/>
+      <c r="F839" s="10"/>
     </row>
     <row r="840">
-      <c r="F840" s="5"/>
+      <c r="F840" s="10"/>
     </row>
     <row r="841">
-      <c r="F841" s="5"/>
+      <c r="F841" s="10"/>
     </row>
     <row r="842">
-      <c r="F842" s="5"/>
+      <c r="F842" s="10"/>
     </row>
     <row r="843">
-      <c r="F843" s="5"/>
+      <c r="F843" s="10"/>
     </row>
     <row r="844">
-      <c r="F844" s="5"/>
+      <c r="F844" s="10"/>
     </row>
     <row r="845">
-      <c r="F845" s="5"/>
+      <c r="F845" s="10"/>
     </row>
     <row r="846">
-      <c r="F846" s="5"/>
+      <c r="F846" s="10"/>
     </row>
     <row r="847">
-      <c r="F847" s="5"/>
+      <c r="F847" s="10"/>
     </row>
     <row r="848">
-      <c r="F848" s="5"/>
+      <c r="F848" s="10"/>
     </row>
     <row r="849">
-      <c r="F849" s="5"/>
+      <c r="F849" s="10"/>
     </row>
     <row r="850">
-      <c r="F850" s="5"/>
+      <c r="F850" s="10"/>
     </row>
     <row r="851">
-      <c r="F851" s="5"/>
+      <c r="F851" s="10"/>
     </row>
     <row r="852">
-      <c r="F852" s="5"/>
+      <c r="F852" s="10"/>
     </row>
     <row r="853">
-      <c r="F853" s="5"/>
+      <c r="F853" s="10"/>
     </row>
     <row r="854">
-      <c r="F854" s="5"/>
+      <c r="F854" s="10"/>
     </row>
     <row r="855">
-      <c r="F855" s="5"/>
+      <c r="F855" s="10"/>
     </row>
     <row r="856">
-      <c r="F856" s="5"/>
+      <c r="F856" s="10"/>
     </row>
     <row r="857">
-      <c r="F857" s="5"/>
+      <c r="F857" s="10"/>
     </row>
     <row r="858">
-      <c r="F858" s="5"/>
+      <c r="F858" s="10"/>
     </row>
     <row r="859">
-      <c r="F859" s="5"/>
+      <c r="F859" s="10"/>
     </row>
     <row r="860">
-      <c r="F860" s="5"/>
+      <c r="F860" s="10"/>
     </row>
     <row r="861">
-      <c r="F861" s="5"/>
+      <c r="F861" s="10"/>
     </row>
     <row r="862">
-      <c r="F862" s="5"/>
+      <c r="F862" s="10"/>
     </row>
     <row r="863">
-      <c r="F863" s="5"/>
+      <c r="F863" s="10"/>
     </row>
     <row r="864">
-      <c r="F864" s="5"/>
+      <c r="F864" s="10"/>
     </row>
     <row r="865">
-      <c r="F865" s="5"/>
+      <c r="F865" s="10"/>
     </row>
     <row r="866">
-      <c r="F866" s="5"/>
+      <c r="F866" s="10"/>
     </row>
     <row r="867">
-      <c r="F867" s="5"/>
+      <c r="F867" s="10"/>
     </row>
     <row r="868">
-      <c r="F868" s="5"/>
+      <c r="F868" s="10"/>
     </row>
     <row r="869">
-      <c r="F869" s="5"/>
+      <c r="F869" s="10"/>
     </row>
     <row r="870">
-      <c r="F870" s="5"/>
+      <c r="F870" s="10"/>
     </row>
     <row r="871">
-      <c r="F871" s="5"/>
+      <c r="F871" s="10"/>
     </row>
     <row r="872">
-      <c r="F872" s="5"/>
+      <c r="F872" s="10"/>
     </row>
     <row r="873">
-      <c r="F873" s="5"/>
+      <c r="F873" s="10"/>
     </row>
     <row r="874">
-      <c r="F874" s="5"/>
+      <c r="F874" s="10"/>
     </row>
     <row r="875">
-      <c r="F875" s="5"/>
+      <c r="F875" s="10"/>
     </row>
     <row r="876">
-      <c r="F876" s="5"/>
+      <c r="F876" s="10"/>
     </row>
     <row r="877">
-      <c r="F877" s="5"/>
+      <c r="F877" s="10"/>
     </row>
     <row r="878">
-      <c r="F878" s="5"/>
+      <c r="F878" s="10"/>
     </row>
     <row r="879">
-      <c r="F879" s="5"/>
+      <c r="F879" s="10"/>
     </row>
     <row r="880">
-      <c r="F880" s="5"/>
+      <c r="F880" s="10"/>
     </row>
     <row r="881">
-      <c r="F881" s="5"/>
+      <c r="F881" s="10"/>
     </row>
     <row r="882">
-      <c r="F882" s="5"/>
+      <c r="F882" s="10"/>
     </row>
     <row r="883">
-      <c r="F883" s="5"/>
+      <c r="F883" s="10"/>
     </row>
     <row r="884">
-      <c r="F884" s="5"/>
+      <c r="F884" s="10"/>
     </row>
     <row r="885">
-      <c r="F885" s="5"/>
+      <c r="F885" s="10"/>
     </row>
     <row r="886">
-      <c r="F886" s="5"/>
+      <c r="F886" s="10"/>
     </row>
     <row r="887">
-      <c r="F887" s="5"/>
+      <c r="F887" s="10"/>
     </row>
     <row r="888">
-      <c r="F888" s="5"/>
+      <c r="F888" s="10"/>
     </row>
     <row r="889">
-      <c r="F889" s="5"/>
+      <c r="F889" s="10"/>
     </row>
     <row r="890">
-      <c r="F890" s="5"/>
+      <c r="F890" s="10"/>
     </row>
     <row r="891">
-      <c r="F891" s="5"/>
+      <c r="F891" s="10"/>
     </row>
     <row r="892">
-      <c r="F892" s="5"/>
+      <c r="F892" s="10"/>
     </row>
     <row r="893">
-      <c r="F893" s="5"/>
+      <c r="F893" s="10"/>
     </row>
     <row r="894">
-      <c r="F894" s="5"/>
+      <c r="F894" s="10"/>
     </row>
     <row r="895">
-      <c r="F895" s="5"/>
+      <c r="F895" s="10"/>
     </row>
     <row r="896">
-      <c r="F896" s="5"/>
+      <c r="F896" s="10"/>
     </row>
     <row r="897">
-      <c r="F897" s="5"/>
+      <c r="F897" s="10"/>
     </row>
     <row r="898">
-      <c r="F898" s="5"/>
+      <c r="F898" s="10"/>
     </row>
     <row r="899">
-      <c r="F899" s="5"/>
+      <c r="F899" s="10"/>
     </row>
     <row r="900">
-      <c r="F900" s="5"/>
+      <c r="F900" s="10"/>
     </row>
     <row r="901">
-      <c r="F901" s="5"/>
+      <c r="F901" s="10"/>
     </row>
     <row r="902">
-      <c r="F902" s="5"/>
+      <c r="F902" s="10"/>
     </row>
     <row r="903">
-      <c r="F903" s="5"/>
+      <c r="F903" s="10"/>
     </row>
     <row r="904">
-      <c r="F904" s="5"/>
+      <c r="F904" s="10"/>
     </row>
     <row r="905">
-      <c r="F905" s="5"/>
+      <c r="F905" s="10"/>
     </row>
     <row r="906">
-      <c r="F906" s="5"/>
+      <c r="F906" s="10"/>
     </row>
     <row r="907">
-      <c r="F907" s="5"/>
+      <c r="F907" s="10"/>
     </row>
     <row r="908">
-      <c r="F908" s="5"/>
+      <c r="F908" s="10"/>
     </row>
     <row r="909">
-      <c r="F909" s="5"/>
+      <c r="F909" s="10"/>
     </row>
     <row r="910">
-      <c r="F910" s="5"/>
+      <c r="F910" s="10"/>
     </row>
     <row r="911">
-      <c r="F911" s="5"/>
+      <c r="F911" s="10"/>
     </row>
     <row r="912">
-      <c r="F912" s="5"/>
+      <c r="F912" s="10"/>
     </row>
     <row r="913">
-      <c r="F913" s="5"/>
+      <c r="F913" s="10"/>
     </row>
     <row r="914">
-      <c r="F914" s="5"/>
+      <c r="F914" s="10"/>
     </row>
     <row r="915">
-      <c r="F915" s="5"/>
+      <c r="F915" s="10"/>
     </row>
     <row r="916">
-      <c r="F916" s="5"/>
+      <c r="F916" s="10"/>
     </row>
     <row r="917">
-      <c r="F917" s="5"/>
+      <c r="F917" s="10"/>
     </row>
     <row r="918">
-      <c r="F918" s="5"/>
+      <c r="F918" s="10"/>
     </row>
     <row r="919">
-      <c r="F919" s="5"/>
+      <c r="F919" s="10"/>
     </row>
     <row r="920">
-      <c r="F920" s="5"/>
+      <c r="F920" s="10"/>
     </row>
     <row r="921">
-      <c r="F921" s="5"/>
+      <c r="F921" s="10"/>
     </row>
     <row r="922">
-      <c r="F922" s="5"/>
+      <c r="F922" s="10"/>
     </row>
     <row r="923">
-      <c r="F923" s="5"/>
+      <c r="F923" s="10"/>
     </row>
     <row r="924">
-      <c r="F924" s="5"/>
+      <c r="F924" s="10"/>
     </row>
     <row r="925">
-      <c r="F925" s="5"/>
+      <c r="F925" s="10"/>
     </row>
     <row r="926">
-      <c r="F926" s="5"/>
+      <c r="F926" s="10"/>
     </row>
     <row r="927">
-      <c r="F927" s="5"/>
+      <c r="F927" s="10"/>
     </row>
     <row r="928">
-      <c r="F928" s="5"/>
+      <c r="F928" s="10"/>
     </row>
     <row r="929">
-      <c r="F929" s="5"/>
+      <c r="F929" s="10"/>
     </row>
     <row r="930">
-      <c r="F930" s="5"/>
+      <c r="F930" s="10"/>
     </row>
     <row r="931">
-      <c r="F931" s="5"/>
+      <c r="F931" s="10"/>
     </row>
     <row r="932">
-      <c r="F932" s="5"/>
+      <c r="F932" s="10"/>
     </row>
     <row r="933">
-      <c r="F933" s="5"/>
+      <c r="F933" s="10"/>
     </row>
     <row r="934">
-      <c r="F934" s="5"/>
+      <c r="F934" s="10"/>
     </row>
     <row r="935">
-      <c r="F935" s="5"/>
+      <c r="F935" s="10"/>
     </row>
     <row r="936">
-      <c r="F936" s="5"/>
+      <c r="F936" s="10"/>
     </row>
     <row r="937">
-      <c r="F937" s="5"/>
+      <c r="F937" s="10"/>
     </row>
     <row r="938">
-      <c r="F938" s="5"/>
+      <c r="F938" s="10"/>
     </row>
     <row r="939">
-      <c r="F939" s="5"/>
+      <c r="F939" s="10"/>
     </row>
     <row r="940">
-      <c r="F940" s="5"/>
+      <c r="F940" s="10"/>
     </row>
     <row r="941">
-      <c r="F941" s="5"/>
+      <c r="F941" s="10"/>
     </row>
     <row r="942">
-      <c r="F942" s="5"/>
+      <c r="F942" s="10"/>
     </row>
     <row r="943">
-      <c r="F943" s="5"/>
+      <c r="F943" s="10"/>
     </row>
     <row r="944">
-      <c r="F944" s="5"/>
+      <c r="F944" s="10"/>
     </row>
     <row r="945">
-      <c r="F945" s="5"/>
+      <c r="F945" s="10"/>
     </row>
     <row r="946">
-      <c r="F946" s="5"/>
+      <c r="F946" s="10"/>
     </row>
     <row r="947">
-      <c r="F947" s="5"/>
+      <c r="F947" s="10"/>
     </row>
     <row r="948">
-      <c r="F948" s="5"/>
+      <c r="F948" s="10"/>
     </row>
     <row r="949">
-      <c r="F949" s="5"/>
+      <c r="F949" s="10"/>
     </row>
     <row r="950">
-      <c r="F950" s="5"/>
+      <c r="F950" s="10"/>
     </row>
     <row r="951">
-      <c r="F951" s="5"/>
+      <c r="F951" s="10"/>
     </row>
     <row r="952">
-      <c r="F952" s="5"/>
+      <c r="F952" s="10"/>
     </row>
     <row r="953">
-      <c r="F953" s="5"/>
+      <c r="F953" s="10"/>
     </row>
     <row r="954">
-      <c r="F954" s="5"/>
+      <c r="F954" s="10"/>
     </row>
     <row r="955">
-      <c r="F955" s="5"/>
+      <c r="F955" s="10"/>
     </row>
     <row r="956">
-      <c r="F956" s="5"/>
+      <c r="F956" s="10"/>
     </row>
     <row r="957">
-      <c r="F957" s="5"/>
+      <c r="F957" s="10"/>
     </row>
     <row r="958">
-      <c r="F958" s="5"/>
+      <c r="F958" s="10"/>
     </row>
     <row r="959">
-      <c r="F959" s="5"/>
+      <c r="F959" s="10"/>
     </row>
     <row r="960">
-      <c r="F960" s="5"/>
+      <c r="F960" s="10"/>
     </row>
     <row r="961">
-      <c r="F961" s="5"/>
+      <c r="F961" s="10"/>
     </row>
     <row r="962">
-      <c r="F962" s="5"/>
+      <c r="F962" s="10"/>
     </row>
     <row r="963">
-      <c r="F963" s="5"/>
+      <c r="F963" s="10"/>
     </row>
     <row r="964">
-      <c r="F964" s="5"/>
+      <c r="F964" s="10"/>
     </row>
     <row r="965">
-      <c r="F965" s="5"/>
+      <c r="F965" s="10"/>
     </row>
     <row r="966">
-      <c r="F966" s="5"/>
+      <c r="F966" s="10"/>
     </row>
     <row r="967">
-      <c r="F967" s="5"/>
+      <c r="F967" s="10"/>
     </row>
     <row r="968">
-      <c r="F968" s="5"/>
+      <c r="F968" s="10"/>
     </row>
     <row r="969">
-      <c r="F969" s="5"/>
+      <c r="F969" s="10"/>
     </row>
     <row r="970">
-      <c r="F970" s="5"/>
+      <c r="F970" s="10"/>
     </row>
     <row r="971">
-      <c r="F971" s="5"/>
+      <c r="F971" s="10"/>
     </row>
     <row r="972">
-      <c r="F972" s="5"/>
+      <c r="F972" s="10"/>
     </row>
     <row r="973">
-      <c r="F973" s="5"/>
+      <c r="F973" s="10"/>
     </row>
     <row r="974">
-      <c r="F974" s="5"/>
+      <c r="F974" s="10"/>
     </row>
     <row r="975">
-      <c r="F975" s="5"/>
+      <c r="F975" s="10"/>
     </row>
     <row r="976">
-      <c r="F976" s="5"/>
+      <c r="F976" s="10"/>
     </row>
     <row r="977">
-      <c r="F977" s="5"/>
+      <c r="F977" s="10"/>
     </row>
     <row r="978">
-      <c r="F978" s="5"/>
+      <c r="F978" s="10"/>
     </row>
     <row r="979">
-      <c r="F979" s="5"/>
+      <c r="F979" s="10"/>
     </row>
     <row r="980">
-      <c r="F980" s="5"/>
+      <c r="F980" s="10"/>
     </row>
     <row r="981">
-      <c r="F981" s="5"/>
+      <c r="F981" s="10"/>
     </row>
     <row r="982">
-      <c r="F982" s="5"/>
+      <c r="F982" s="10"/>
     </row>
     <row r="983">
-      <c r="F983" s="5"/>
+      <c r="F983" s="10"/>
     </row>
     <row r="984">
-      <c r="F984" s="5"/>
+      <c r="F984" s="10"/>
     </row>
     <row r="985">
-      <c r="F985" s="5"/>
+      <c r="F985" s="10"/>
     </row>
     <row r="986">
-      <c r="F986" s="5"/>
+      <c r="F986" s="10"/>
     </row>
     <row r="987">
-      <c r="F987" s="5"/>
+      <c r="F987" s="10"/>
     </row>
     <row r="988">
-      <c r="F988" s="5"/>
+      <c r="F988" s="10"/>
     </row>
     <row r="989">
-      <c r="F989" s="5"/>
+      <c r="F989" s="10"/>
     </row>
     <row r="990">
-      <c r="F990" s="5"/>
+      <c r="F990" s="10"/>
     </row>
     <row r="991">
-      <c r="F991" s="5"/>
+      <c r="F991" s="10"/>
     </row>
     <row r="992">
-      <c r="F992" s="5"/>
+      <c r="F992" s="10"/>
     </row>
     <row r="993">
-      <c r="F993" s="5"/>
+      <c r="F993" s="10"/>
     </row>
     <row r="994">
-      <c r="F994" s="5"/>
+      <c r="F994" s="10"/>
     </row>
     <row r="995">
-      <c r="F995" s="5"/>
+      <c r="F995" s="10"/>
     </row>
     <row r="996">
-      <c r="F996" s="5"/>
+      <c r="F996" s="10"/>
     </row>
     <row r="997">
-      <c r="F997" s="5"/>
+      <c r="F997" s="10"/>
     </row>
     <row r="998">
-      <c r="F998" s="5"/>
+      <c r="F998" s="10"/>
     </row>
     <row r="999">
-      <c r="F999" s="5"/>
+      <c r="F999" s="10"/>
     </row>
     <row r="1000">
-      <c r="F1000" s="5"/>
+      <c r="F1000" s="10"/>
     </row>
     <row r="1001">
-      <c r="F1001" s="5"/>
+      <c r="F1001" s="10"/>
     </row>
     <row r="1002">
-      <c r="F1002" s="5"/>
+      <c r="F1002" s="10"/>
     </row>
     <row r="1003">
-      <c r="F1003" s="5"/>
+      <c r="F1003" s="10"/>
     </row>
     <row r="1004">
-      <c r="F1004" s="5"/>
+      <c r="F1004" s="10"/>
     </row>
     <row r="1005">
-      <c r="F1005" s="5"/>
+      <c r="F1005" s="10"/>
     </row>
     <row r="1006">
-      <c r="F1006" s="5"/>
+      <c r="F1006" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3428,87 +3476,87 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="15"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3523,25 +3571,25 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
+      <c r="B1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="14">
-        <v>2.016110801E9</v>
+      <c r="A2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="16">
+        <v>2.016120801E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>